<commit_message>
feat: betting tracker is ready!
</commit_message>
<xml_diff>
--- a/betting_tracker.xlsx
+++ b/betting_tracker.xlsx
@@ -556,27 +556,27 @@
       </c>
       <c r="D1" s="16" t="inlineStr">
         <is>
+          <t>betting_line</t>
+        </is>
+      </c>
+      <c r="E1" s="16" t="inlineStr">
+        <is>
           <t>goalie_id</t>
         </is>
       </c>
-      <c r="E1" s="16" t="inlineStr">
+      <c r="F1" s="16" t="inlineStr">
         <is>
           <t>team_abbrev</t>
         </is>
       </c>
-      <c r="F1" s="16" t="inlineStr">
+      <c r="G1" s="16" t="inlineStr">
         <is>
           <t>opponent_team</t>
         </is>
       </c>
-      <c r="G1" s="16" t="inlineStr">
+      <c r="H1" s="16" t="inlineStr">
         <is>
           <t>is_home</t>
-        </is>
-      </c>
-      <c r="H1" s="16" t="inlineStr">
-        <is>
-          <t>betting_line</t>
         </is>
       </c>
       <c r="I1" s="16" t="inlineStr">
@@ -644,26 +644,22 @@
       <c r="B2" t="n">
         <v>2025020657</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>DAL</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>MTL</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -689,26 +685,22 @@
       <c r="B3" t="n">
         <v>2025020657</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
         <is>
           <t>MTL</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>DAL</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0</v>
       </c>
-      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
@@ -734,26 +726,22 @@
       <c r="B4" t="n">
         <v>2025020658</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>CBJ</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>PIT</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>1</v>
       </c>
-      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -779,26 +767,22 @@
       <c r="B5" t="n">
         <v>2025020658</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
         <is>
           <t>PIT</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>CBJ</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>0</v>
       </c>
-      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -824,49 +808,27 @@
       <c r="B6" t="n">
         <v>2025020659</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Tarasov</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>8480193</v>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
         <is>
           <t>FLA</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>COL</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>1</v>
       </c>
-      <c r="H6" t="n">
-        <v>25.5</v>
-      </c>
-      <c r="I6" t="n">
-        <v>25</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.4832989275455475</v>
-      </c>
-      <c r="K6" t="n">
-        <v>3.340214490890503</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>50-55%</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
@@ -887,47 +849,27 @@
       <c r="B7" t="n">
         <v>2025020659</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>8480193</v>
-      </c>
-      <c r="E7" t="inlineStr">
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
         <is>
           <t>COL</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>FLA</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0</v>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>25</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.4832989275455475</v>
-      </c>
-      <c r="K7" t="n">
-        <v>3.340214490890503</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>50-55%</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
@@ -954,26 +896,26 @@
         </is>
       </c>
       <c r="D8" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="E8" t="n">
         <v>8474596</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>NJD</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>25.5</v>
-      </c>
-      <c r="I8" t="n">
-        <v>25</v>
       </c>
       <c r="J8" t="n">
         <v>0.5094840526580811</v>
@@ -1017,32 +959,32 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>8474596</v>
-      </c>
-      <c r="E9" t="inlineStr">
+        <v>23.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8483548</v>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>CAR</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>NJD</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>0</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>23.5</v>
       </c>
-      <c r="I9" t="n">
-        <v>25</v>
-      </c>
       <c r="J9" t="n">
-        <v>0.5094840526580811</v>
+        <v>0.4905944764614105</v>
       </c>
       <c r="K9" t="n">
-        <v>1.896810531616211</v>
+        <v>1.881104707717896</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -1080,26 +1022,26 @@
         </is>
       </c>
       <c r="D10" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="E10" t="n">
         <v>8482821</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>CHI</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>VGK</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>1</v>
       </c>
-      <c r="H10" t="n">
-        <v>25.5</v>
-      </c>
       <c r="I10" t="n">
-        <v>25</v>
+        <v>25.39999961853027</v>
       </c>
       <c r="J10" t="n">
         <v>0.4777129590511322</v>
@@ -1137,47 +1079,27 @@
       <c r="B11" t="n">
         <v>2025020661</v>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>8482821</v>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
         <is>
           <t>VGK</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>CHI</t>
         </is>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>0</v>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
-        <v>25</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.4777129590511322</v>
-      </c>
-      <c r="K11" t="n">
-        <v>4.45740795135498</v>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>50-55%</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
@@ -1238,7 +1160,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>2026-01-04 15:13:01</t>
+          <t>2026-01-04 16:16:51</t>
         </is>
       </c>
       <c r="C3" s="11" t="n"/>

</xml_diff>

<commit_message>
feat: best one yet
</commit_message>
<xml_diff>
--- a/betting_tracker.xlsx
+++ b/betting_tracker.xlsx
@@ -55,6 +55,12 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="14"/>
     </font>
@@ -67,12 +73,8 @@
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -84,14 +86,8 @@
         <fgColor rgb="FF4472c4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004472C4"/>
-        <bgColor rgb="004472C4"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -137,6 +133,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -146,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -184,22 +195,25 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -208,10 +222,13 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -220,11 +237,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,14 +614,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="24" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="26" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="18" t="inlineStr">
+      <c r="A1" s="19" t="inlineStr">
         <is>
           <t>BETTING PERFORMANCE SUMMARY</t>
         </is>
@@ -644,7 +658,7 @@
       <c r="E4" s="5" t="n"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="22" t="inlineStr">
+      <c r="A5" s="24" t="inlineStr">
         <is>
           <t>OVERALL PERFORMANCE</t>
         </is>
@@ -734,10 +748,8 @@
           <t>Total Profit/Loss</t>
         </is>
       </c>
-      <c r="B12" s="5" t="inlineStr">
-        <is>
-          <t>-3.41</t>
-        </is>
+      <c r="B12" s="5" t="n">
+        <v>-3.41</v>
       </c>
       <c r="C12" s="5" t="n"/>
       <c r="D12" s="5" t="n"/>
@@ -773,7 +785,7 @@
       <c r="E15" s="5" t="n"/>
     </row>
     <row r="16" ht="20.25" customHeight="1">
-      <c r="A16" s="22" t="inlineStr">
+      <c r="A16" s="24" t="inlineStr">
         <is>
           <t>PERFORMANCE BY CONFIDENCE LEVEL</t>
         </is>
@@ -784,27 +796,27 @@
       <c r="E16" s="5" t="n"/>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="A17" s="19" t="inlineStr">
+      <c r="A17" s="20" t="inlineStr">
         <is>
           <t>Confidence</t>
         </is>
       </c>
-      <c r="B17" s="20" t="inlineStr">
+      <c r="B17" s="21" t="inlineStr">
         <is>
           <t>Bets</t>
         </is>
       </c>
-      <c r="C17" s="20" t="inlineStr">
+      <c r="C17" s="21" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="D17" s="19" t="inlineStr">
+      <c r="D17" s="20" t="inlineStr">
         <is>
           <t>Win Rate</t>
         </is>
       </c>
-      <c r="E17" s="20" t="inlineStr">
+      <c r="E17" s="21" t="inlineStr">
         <is>
           <t>ROI %</t>
         </is>
@@ -822,7 +834,7 @@
       <c r="C18" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D18" s="23" t="inlineStr">
+      <c r="D18" s="25" t="inlineStr">
         <is>
           <t>50.0%</t>
         </is>
@@ -845,7 +857,7 @@
       <c r="C19" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="D19" s="23" t="inlineStr">
+      <c r="D19" s="25" t="inlineStr">
         <is>
           <t>38.5%</t>
         </is>
@@ -868,7 +880,7 @@
       <c r="C20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="23" t="inlineStr">
+      <c r="D20" s="25" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
@@ -891,7 +903,7 @@
       <c r="C21" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D21" s="23" t="inlineStr">
+      <c r="D21" s="25" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
@@ -914,7 +926,7 @@
       <c r="C22" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D22" s="23" t="inlineStr">
+      <c r="D22" s="25" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
@@ -937,7 +949,7 @@
       <c r="C23" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D23" s="23" t="inlineStr">
+      <c r="D23" s="25" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
@@ -971,15 +983,15 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
@@ -987,9 +999,9 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="16" max="16"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="17" max="17"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="18" max="18"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="19" max="19"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="20" max="20"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="20" max="20"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="21" max="21"/>
   </cols>
   <sheetData>
@@ -1821,25 +1833,25 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12.005" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="12.005" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="12.005" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
     <col width="18.005" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.005" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
-    <col width="12.005" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="12.005" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="12.005" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
     <col width="15.005" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="10.005" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="10.005" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
     <col width="15.005" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
     <col width="12.005" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
     <col width="14.005" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
     <col width="16.005" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
     <col width="15.005" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
-    <col width="12.005" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
+    <col width="12.005" bestFit="1" customWidth="1" style="22" min="16" max="16"/>
     <col width="14.005" bestFit="1" customWidth="1" style="7" min="17" max="17"/>
-    <col width="13.005" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
+    <col width="13.005" bestFit="1" customWidth="1" style="22" min="18" max="18"/>
     <col width="10.005" bestFit="1" customWidth="1" style="7" min="19" max="19"/>
-    <col width="12.005" bestFit="1" customWidth="1" style="8" min="20" max="20"/>
+    <col width="12.005" bestFit="1" customWidth="1" style="22" min="20" max="20"/>
     <col width="30.005" bestFit="1" customWidth="1" style="7" min="21" max="21"/>
   </cols>
   <sheetData>
@@ -2702,11 +2714,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30.005" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="20.005" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="20.005" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="18" t="inlineStr">
+      <c r="A1" s="19" t="inlineStr">
         <is>
           <t>BETTING TRACKER SETTINGS</t>
         </is>
@@ -2718,12 +2730,12 @@
       <c r="B2" s="5" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="19" t="inlineStr">
+      <c r="A3" s="20" t="inlineStr">
         <is>
           <t>Setting</t>
         </is>
       </c>
-      <c r="B3" s="20" t="inlineStr">
+      <c r="B3" s="21" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
@@ -2823,137 +2835,113 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="14" customWidth="1" min="13" max="13"/>
-    <col width="16" customWidth="1" min="14" max="14"/>
-    <col width="15" customWidth="1" min="15" max="15"/>
-    <col width="12" customWidth="1" min="16" max="16"/>
-    <col width="14" customWidth="1" min="17" max="17"/>
-    <col width="13" customWidth="1" min="18" max="18"/>
-    <col width="10" customWidth="1" min="19" max="19"/>
-    <col width="12" customWidth="1" min="20" max="20"/>
-    <col width="30" customWidth="1" min="21" max="21"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="26" t="inlineStr">
+      <c r="A1" s="27" t="inlineStr">
         <is>
           <t>game_date</t>
         </is>
       </c>
-      <c r="B1" s="26" t="inlineStr">
+      <c r="B1" s="27" t="inlineStr">
         <is>
           <t>game_id</t>
         </is>
       </c>
-      <c r="C1" s="26" t="inlineStr">
+      <c r="C1" s="27" t="inlineStr">
         <is>
           <t>goalie_name</t>
         </is>
       </c>
-      <c r="D1" s="26" t="inlineStr">
+      <c r="D1" s="27" t="inlineStr">
         <is>
           <t>betting_line</t>
         </is>
       </c>
-      <c r="E1" s="26" t="inlineStr">
+      <c r="E1" s="27" t="inlineStr">
         <is>
           <t>line_over</t>
         </is>
       </c>
-      <c r="F1" s="26" t="inlineStr">
+      <c r="F1" s="27" t="inlineStr">
         <is>
           <t>line_under</t>
         </is>
       </c>
-      <c r="G1" s="26" t="inlineStr">
+      <c r="G1" s="27" t="inlineStr">
         <is>
           <t>goalie_id</t>
         </is>
       </c>
-      <c r="H1" s="26" t="inlineStr">
+      <c r="H1" s="27" t="inlineStr">
         <is>
           <t>team_abbrev</t>
         </is>
       </c>
-      <c r="I1" s="26" t="inlineStr">
+      <c r="I1" s="27" t="inlineStr">
         <is>
           <t>opponent_team</t>
         </is>
       </c>
-      <c r="J1" s="26" t="inlineStr">
+      <c r="J1" s="27" t="inlineStr">
         <is>
           <t>is_home</t>
         </is>
       </c>
-      <c r="K1" s="26" t="inlineStr">
+      <c r="K1" s="27" t="inlineStr">
         <is>
           <t>predicted_saves</t>
         </is>
       </c>
-      <c r="L1" s="26" t="inlineStr">
+      <c r="L1" s="27" t="inlineStr">
         <is>
           <t>prob_over</t>
         </is>
       </c>
-      <c r="M1" s="26" t="inlineStr">
+      <c r="M1" s="27" t="inlineStr">
         <is>
           <t>confidence_pct</t>
         </is>
       </c>
-      <c r="N1" s="26" t="inlineStr">
+      <c r="N1" s="27" t="inlineStr">
         <is>
           <t>confidence_bucket</t>
         </is>
       </c>
-      <c r="O1" s="26" t="inlineStr">
+      <c r="O1" s="27" t="inlineStr">
         <is>
           <t>recommendation</t>
         </is>
       </c>
-      <c r="P1" s="26" t="inlineStr">
+      <c r="P1" s="27" t="inlineStr">
         <is>
           <t>bet_amount</t>
         </is>
       </c>
-      <c r="Q1" s="26" t="inlineStr">
+      <c r="Q1" s="27" t="inlineStr">
         <is>
           <t>bet_selection</t>
         </is>
       </c>
-      <c r="R1" s="26" t="inlineStr">
+      <c r="R1" s="27" t="inlineStr">
         <is>
           <t>actual_saves</t>
         </is>
       </c>
-      <c r="S1" s="26" t="inlineStr">
+      <c r="S1" s="27" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="T1" s="26" t="inlineStr">
+      <c r="T1" s="27" t="inlineStr">
         <is>
           <t>profit_loss</t>
         </is>
       </c>
-      <c r="U1" s="26" t="inlineStr">
+      <c r="U1" s="27" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
@@ -2968,10 +2956,23 @@
       <c r="B2" t="n">
         <v>2025020716</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ellis</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-102</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-129</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8481551</v>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>BUF</t>
@@ -2985,11 +2986,25 @@
       <c r="J2" t="n">
         <v>1</v>
       </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.5060381889343262</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1.207637786865234</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
@@ -3010,10 +3025,23 @@
       <c r="B3" t="n">
         <v>2025020716</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>bobrovsky</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-108</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-121</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8475683</v>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>FLA</t>
@@ -3027,11 +3055,25 @@
       <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>23.60000038146973</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.5227136611938477</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4.542732238769531</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
@@ -3052,10 +3094,23 @@
       <c r="B4" t="n">
         <v>2025020717</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Gibson</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-103</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-127</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8476434</v>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
           <t>DET</t>
@@ -3069,11 +3124,25 @@
       <c r="J4" t="n">
         <v>1</v>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.5014620423316956</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.2924084663391113</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
@@ -3094,10 +3163,23 @@
       <c r="B5" t="n">
         <v>2025020717</v>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>andersen</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-130</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8475883</v>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
           <t>CAR</t>
@@ -3111,11 +3193,25 @@
       <c r="J5" t="n">
         <v>0</v>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>21.79999923706055</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.5524033904075623</v>
+      </c>
+      <c r="M5" t="n">
+        <v>10.48067855834961</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>55-60%</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>OVER</t>
+        </is>
+      </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
@@ -3136,10 +3232,23 @@
       <c r="B6" t="n">
         <v>2025020718</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>quick</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-103</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-127</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8471734</v>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>NYR</t>
@@ -3153,11 +3262,25 @@
       <c r="J6" t="n">
         <v>1</v>
       </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="K6" t="n">
+        <v>22.89999961853027</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5868213176727295</v>
+      </c>
+      <c r="M6" t="n">
+        <v>17.3642635345459</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>55-60%</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>OVER</t>
+        </is>
+      </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
@@ -3178,10 +3301,23 @@
       <c r="B7" t="n">
         <v>2025020718</v>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>grubauer</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-110</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-118</v>
+      </c>
+      <c r="G7" t="n">
+        <v>8475831</v>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
           <t>SEA</t>
@@ -3195,11 +3331,25 @@
       <c r="J7" t="n">
         <v>0</v>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.5074939131736755</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.498782634735107</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
@@ -3220,10 +3370,23 @@
       <c r="B8" t="n">
         <v>2025020719</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>vladar</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>106</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-137</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8478435</v>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
           <t>PHI</t>
@@ -3237,11 +3400,25 @@
       <c r="J8" t="n">
         <v>1</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>23</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.5969618558883667</v>
+      </c>
+      <c r="M8" t="n">
+        <v>19.39237213134766</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>55-60%</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>OVER</t>
+        </is>
+      </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
@@ -3262,10 +3439,23 @@
       <c r="B9" t="n">
         <v>2025020719</v>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>johansson</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-122</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-107</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8477992</v>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>TBL</t>
@@ -3279,11 +3469,25 @@
       <c r="J9" t="n">
         <v>0</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>22.70000076293945</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.5488682389259338</v>
+      </c>
+      <c r="M9" t="n">
+        <v>9.773647308349609</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
@@ -3304,10 +3508,23 @@
       <c r="B10" t="n">
         <v>2025020720</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>dobes</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-102</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-129</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8482487</v>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
           <t>MTL</t>
@@ -3321,11 +3538,25 @@
       <c r="J10" t="n">
         <v>1</v>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>22.89999961853027</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.5871408581733704</v>
+      </c>
+      <c r="M10" t="n">
+        <v>17.42817115783691</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>55-60%</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>OVER</t>
+        </is>
+      </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
@@ -3346,10 +3577,23 @@
       <c r="B11" t="n">
         <v>2025020720</v>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>tolopilo</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-108</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-121</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8484268</v>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t>VAN</t>
@@ -3363,11 +3607,25 @@
       <c r="J11" t="n">
         <v>0</v>
       </c>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="K11" t="n">
+        <v>23.70000076293945</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.5326730012893677</v>
+      </c>
+      <c r="M11" t="n">
+        <v>6.534600257873535</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
@@ -3388,10 +3646,23 @@
       <c r="B12" t="n">
         <v>2025020721</v>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>wallstedt</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-113</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-115</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8482661</v>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
           <t>MIN</t>
@@ -3405,17 +3676,27 @@
       <c r="J12" t="n">
         <v>1</v>
       </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="K12" t="n">
+        <v>25.70000076293945</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.5452720522880554</v>
+      </c>
+      <c r="M12" t="n">
+        <v>9.054410934448242</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
+      <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -3430,10 +3711,23 @@
       <c r="B13" t="n">
         <v>2025020721</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>markstrom</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-117</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-112</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8474593</v>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
           <t>NJD</t>
@@ -3447,17 +3741,27 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>23.60000038146973</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.5228213667869568</v>
+      </c>
+      <c r="M13" t="n">
+        <v>4.564273357391357</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
+      <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
@@ -3472,10 +3776,23 @@
       <c r="B14" t="n">
         <v>2025020722</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>knight</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-114</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-114</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8481519</v>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
           <t>CHI</t>
@@ -3489,17 +3806,27 @@
       <c r="J14" t="n">
         <v>1</v>
       </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.5004028081893921</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.08056163787841797</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
+      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
@@ -3514,10 +3841,23 @@
       <c r="B15" t="n">
         <v>2025020722</v>
       </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ingram</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-113</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-115</v>
+      </c>
+      <c r="G15" t="n">
+        <v>8478971</v>
+      </c>
       <c r="H15" t="inlineStr">
         <is>
           <t>EDM</t>
@@ -3531,17 +3871,27 @@
       <c r="J15" t="n">
         <v>0</v>
       </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
+      <c r="K15" t="n">
+        <v>21.79999923706055</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.5661694407463074</v>
+      </c>
+      <c r="M15" t="n">
+        <v>13.23388862609863</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>55-60%</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>OVER</t>
+        </is>
+      </c>
       <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
+      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
@@ -3556,10 +3906,23 @@
       <c r="B16" t="n">
         <v>2025020723</v>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>miner</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-130</v>
+      </c>
+      <c r="F16" t="n">
+        <v>100</v>
+      </c>
+      <c r="G16" t="n">
+        <v>8481529</v>
+      </c>
       <c r="H16" t="inlineStr">
         <is>
           <t>COL</t>
@@ -3573,17 +3936,27 @@
       <c r="J16" t="n">
         <v>1</v>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>21.79999923706055</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.5536573529243469</v>
+      </c>
+      <c r="M16" t="n">
+        <v>10.73147010803223</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>55-60%</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
@@ -3598,10 +3971,23 @@
       <c r="B17" t="n">
         <v>2025020723</v>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>woll</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-125</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-104</v>
+      </c>
+      <c r="G17" t="n">
+        <v>8479361</v>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
           <t>TOR</t>
@@ -3615,17 +4001,27 @@
       <c r="J17" t="n">
         <v>0</v>
       </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+      <c r="K17" t="n">
+        <v>28.39999961853027</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.4855145514011383</v>
+      </c>
+      <c r="M17" t="n">
+        <v>2.897089719772339</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
+      <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
@@ -3640,10 +4036,23 @@
       <c r="B18" t="n">
         <v>2025020724</v>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Kuemper</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>106</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-137</v>
+      </c>
+      <c r="G18" t="n">
+        <v>8475311</v>
+      </c>
       <c r="H18" t="inlineStr">
         <is>
           <t>LAK</t>
@@ -3657,17 +4066,27 @@
       <c r="J18" t="n">
         <v>1</v>
       </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>22.79999923706055</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.5581576228141785</v>
+      </c>
+      <c r="M18" t="n">
+        <v>11.63152503967285</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>55-60%</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>OVER</t>
+        </is>
+      </c>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
@@ -3682,10 +4101,23 @@
       <c r="B19" t="n">
         <v>2025020724</v>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>oettinger</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-104</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-125</v>
+      </c>
+      <c r="G19" t="n">
+        <v>8479979</v>
+      </c>
       <c r="H19" t="inlineStr">
         <is>
           <t>DAL</t>
@@ -3699,17 +4131,27 @@
       <c r="J19" t="n">
         <v>0</v>
       </c>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+      <c r="K19" t="n">
+        <v>24.60000038146973</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.5200075507164001</v>
+      </c>
+      <c r="M19" t="n">
+        <v>4.001510143280029</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
+      <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -3723,7 +4165,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:U11"/>
@@ -3733,684 +4175,777 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="16" max="16"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="17" max="17"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="18" max="18"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="19" max="19"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="20" max="20"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="21" max="21"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="25" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>game_date</t>
         </is>
       </c>
-      <c r="B1" s="25" t="inlineStr">
+      <c r="B1" s="11" t="inlineStr">
         <is>
           <t>game_id</t>
         </is>
       </c>
-      <c r="C1" s="25" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>goalie_name</t>
         </is>
       </c>
-      <c r="D1" s="25" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>betting_line</t>
         </is>
       </c>
-      <c r="E1" s="25" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>line_over</t>
         </is>
       </c>
-      <c r="F1" s="25" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t>line_under</t>
         </is>
       </c>
-      <c r="G1" s="25" t="inlineStr">
+      <c r="G1" s="11" t="inlineStr">
         <is>
           <t>goalie_id</t>
         </is>
       </c>
-      <c r="H1" s="25" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>team_abbrev</t>
         </is>
       </c>
-      <c r="I1" s="25" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>opponent_team</t>
         </is>
       </c>
-      <c r="J1" s="25" t="inlineStr">
+      <c r="J1" s="11" t="inlineStr">
         <is>
           <t>is_home</t>
         </is>
       </c>
-      <c r="K1" s="25" t="inlineStr">
+      <c r="K1" s="12" t="inlineStr">
         <is>
           <t>predicted_saves</t>
         </is>
       </c>
-      <c r="L1" s="25" t="inlineStr">
+      <c r="L1" s="12" t="inlineStr">
         <is>
           <t>prob_over</t>
         </is>
       </c>
-      <c r="M1" s="25" t="inlineStr">
+      <c r="M1" s="12" t="inlineStr">
         <is>
           <t>confidence_pct</t>
         </is>
       </c>
-      <c r="N1" s="25" t="inlineStr">
+      <c r="N1" s="10" t="inlineStr">
         <is>
           <t>confidence_bucket</t>
         </is>
       </c>
-      <c r="O1" s="25" t="inlineStr">
+      <c r="O1" s="10" t="inlineStr">
         <is>
           <t>recommendation</t>
         </is>
       </c>
-      <c r="P1" s="25" t="inlineStr">
+      <c r="P1" s="11" t="inlineStr">
         <is>
           <t>bet_amount</t>
         </is>
       </c>
-      <c r="Q1" s="25" t="inlineStr">
+      <c r="Q1" s="10" t="inlineStr">
         <is>
           <t>bet_selection</t>
         </is>
       </c>
-      <c r="R1" s="25" t="inlineStr">
+      <c r="R1" s="11" t="inlineStr">
         <is>
           <t>actual_saves</t>
         </is>
       </c>
-      <c r="S1" s="25" t="inlineStr">
+      <c r="S1" s="10" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="T1" s="25" t="inlineStr">
+      <c r="T1" s="11" t="inlineStr">
         <is>
           <t>profit_loss</t>
         </is>
       </c>
-      <c r="U1" s="25" t="inlineStr">
+      <c r="U1" s="10" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="5" t="n">
         <v>2025020711</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="C2" s="7" t="n"/>
+      <c r="D2" s="6" t="n"/>
+      <c r="E2" s="5" t="n"/>
+      <c r="F2" s="5" t="n"/>
+      <c r="G2" s="5" t="n"/>
+      <c r="H2" s="7" t="inlineStr">
         <is>
           <t>WPG</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="7" t="inlineStr">
         <is>
           <t>NJD</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="J2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="K2" s="6" t="n"/>
+      <c r="L2" s="6" t="n"/>
+      <c r="M2" s="6" t="n"/>
+      <c r="N2" s="7" t="n"/>
+      <c r="O2" s="7" t="n"/>
+      <c r="P2" s="5" t="n"/>
+      <c r="Q2" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="R2" s="5" t="n"/>
+      <c r="S2" s="7" t="n"/>
+      <c r="T2" s="5" t="n"/>
+      <c r="U2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="5" t="n">
         <v>2025020711</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="C3" s="7" t="n"/>
+      <c r="D3" s="6" t="n"/>
+      <c r="E3" s="5" t="n"/>
+      <c r="F3" s="5" t="n"/>
+      <c r="G3" s="5" t="n"/>
+      <c r="H3" s="7" t="inlineStr">
         <is>
           <t>NJD</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="7" t="inlineStr">
         <is>
           <t>WPG</t>
         </is>
       </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="inlineStr">
+      <c r="J3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6" t="n"/>
+      <c r="L3" s="6" t="n"/>
+      <c r="M3" s="6" t="n"/>
+      <c r="N3" s="7" t="n"/>
+      <c r="O3" s="7" t="n"/>
+      <c r="P3" s="5" t="n"/>
+      <c r="Q3" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="R3" s="5" t="n"/>
+      <c r="S3" s="7" t="n"/>
+      <c r="T3" s="5" t="n"/>
+      <c r="U3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="5" t="n">
         <v>2025020712</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="7" t="inlineStr">
         <is>
           <t>korpisalo</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="6" t="n">
         <v>25.5</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="5" t="n">
         <v>106</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" s="5" t="n">
         <v>-137</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" s="5" t="n">
         <v>8476914</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="7" t="inlineStr">
         <is>
           <t>BOS</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" s="7" t="inlineStr">
         <is>
           <t>PIT</t>
         </is>
       </c>
-      <c r="J4" t="n">
+      <c r="J4" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4" s="6" t="n">
         <v>25.60000038146973</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4" s="6" t="n">
         <v>0.5174108147621155</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4" s="6" t="n">
         <v>3.482162952423096</v>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="N4" s="7" t="inlineStr">
         <is>
           <t>50-55%</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="O4" s="7" t="inlineStr">
         <is>
           <t>OVER</t>
         </is>
       </c>
-      <c r="P4" t="n">
+      <c r="P4" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="Q4" s="7" t="inlineStr">
         <is>
           <t>OVER</t>
         </is>
       </c>
-      <c r="R4" t="n">
+      <c r="R4" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="S4" s="7" t="inlineStr">
         <is>
           <t>WIN</t>
         </is>
       </c>
-      <c r="T4" t="n">
+      <c r="T4" s="6" t="n">
         <v>1.06</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="U4" s="7" t="n"/>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="5" t="n">
         <v>2025020712</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="7" t="inlineStr">
         <is>
           <t>skinner</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="6" t="n">
         <v>23.5</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="5" t="n">
         <v>-104</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="5" t="n">
         <v>-118</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="5" t="n">
         <v>8479973</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="7" t="inlineStr">
         <is>
           <t>PIT</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="7" t="inlineStr">
         <is>
           <t>BOS</t>
         </is>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
+      <c r="J5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6" t="n">
         <v>23.60000038146973</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5" s="6" t="n">
         <v>0.5104933977127075</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" s="6" t="n">
         <v>2.098679542541504</v>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="N5" s="7" t="inlineStr">
         <is>
           <t>50-55%</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
+      <c r="O5" s="7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="P5" s="5" t="n"/>
+      <c r="Q5" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="R5" t="n">
+      <c r="R5" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="S5" s="7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="T5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="7" t="n"/>
+    </row>
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="5" t="n">
         <v>2025020713</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="7" t="inlineStr">
         <is>
           <t>Annunen</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="6" t="n">
         <v>23.5</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="5" t="n">
         <v>-118</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="5" t="n">
         <v>-110</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="5" t="n">
         <v>8481020</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="7" t="inlineStr">
         <is>
           <t>NSH</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" s="7" t="inlineStr">
         <is>
           <t>WSH</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6" s="6" t="n">
         <v>23.5</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6" s="6" t="n">
         <v>0.5050497055053711</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6" s="6" t="n">
         <v>1.009941101074219</v>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="N6" s="7" t="inlineStr">
         <is>
           <t>50-55%</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
+      <c r="O6" s="7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="P6" s="5" t="n"/>
+      <c r="Q6" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="R6" t="n">
+      <c r="R6" s="5" t="n">
         <v>28</v>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="S6" s="7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="T6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="7" t="n"/>
+    </row>
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="5" t="n">
         <v>2025020713</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="7" t="inlineStr">
         <is>
           <t>lindgren</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="6" t="n">
         <v>24.5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="5" t="n">
         <v>-124</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="5" t="n">
         <v>-106</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="5" t="n">
         <v>8479292</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="7" t="inlineStr">
         <is>
           <t>WSH</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" s="7" t="inlineStr">
         <is>
           <t>NSH</t>
         </is>
       </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
+      <c r="J7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6" t="n">
         <v>24.29999923706055</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L7" s="6" t="n">
         <v>0.4668174088001251</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M7" s="6" t="n">
         <v>6.636518478393555</v>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="N7" s="7" t="inlineStr">
         <is>
           <t>50-55%</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
+      <c r="O7" s="7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="P7" s="5" t="n"/>
+      <c r="Q7" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="R7" t="n">
+      <c r="R7" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
-      <c r="T7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="S7" s="7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="T7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="7" t="n"/>
+    </row>
+    <row r="8" ht="18.75" customHeight="1">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="5" t="n">
         <v>2025020714</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="C8" s="7" t="n"/>
+      <c r="D8" s="6" t="n"/>
+      <c r="E8" s="5" t="n"/>
+      <c r="F8" s="5" t="n"/>
+      <c r="G8" s="5" t="n"/>
+      <c r="H8" s="7" t="inlineStr">
         <is>
           <t>UTA</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" s="7" t="inlineStr">
         <is>
           <t>CBJ</t>
         </is>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="K8" s="6" t="n"/>
+      <c r="L8" s="6" t="n"/>
+      <c r="M8" s="6" t="n"/>
+      <c r="N8" s="7" t="n"/>
+      <c r="O8" s="7" t="n"/>
+      <c r="P8" s="5" t="n"/>
+      <c r="Q8" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="R8" s="5" t="n"/>
+      <c r="S8" s="7" t="n"/>
+      <c r="T8" s="5" t="n"/>
+      <c r="U8" s="7" t="n"/>
+    </row>
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="5" t="n">
         <v>2025020714</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="7" t="inlineStr">
         <is>
           <t>greaves</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="6" t="n">
         <v>26.5</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="5" t="n">
         <v>-106</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="5" t="n">
         <v>-124</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="5" t="n">
         <v>8482982</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" s="7" t="inlineStr">
         <is>
           <t>CBJ</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I9" s="7" t="inlineStr">
         <is>
           <t>UTA</t>
         </is>
       </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
+      <c r="J9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6" t="n">
         <v>26.39999961853027</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L9" s="6" t="n">
         <v>0.4883530735969543</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M9" s="6" t="n">
         <v>2.329385280609131</v>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="N9" s="7" t="inlineStr">
         <is>
           <t>50-55%</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
+      <c r="O9" s="7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="P9" s="5" t="n"/>
+      <c r="Q9" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="R9" t="n">
+      <c r="R9" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>NO BET</t>
-        </is>
-      </c>
-      <c r="T9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="S9" s="7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="T9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="18.75" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="5" t="n">
         <v>2025020715</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="7" t="inlineStr">
         <is>
           <t>askarov</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="6" t="n">
         <v>25.5</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="5" t="n">
         <v>-122</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="5" t="n">
         <v>-107</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" s="5" t="n">
         <v>8482137</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H10" s="7" t="inlineStr">
         <is>
           <t>SJS</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" s="7" t="inlineStr">
         <is>
           <t>VGK</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="J10" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10" s="6" t="n">
         <v>25.20000076293945</v>
       </c>
-      <c r="L10" t="n">
+      <c r="L10" s="6" t="n">
         <v>0.4438229203224182</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M10" s="6" t="n">
         <v>11.23541641235352</v>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="N10" s="7" t="inlineStr">
         <is>
           <t>55-60%</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="O10" s="7" t="inlineStr">
         <is>
           <t>UNDER</t>
         </is>
       </c>
-      <c r="P10" t="n">
+      <c r="P10" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="Q10" s="7" t="inlineStr">
         <is>
           <t>UNDER</t>
         </is>
       </c>
-      <c r="R10" t="n">
+      <c r="R10" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="S10" s="7" t="inlineStr">
         <is>
           <t>LOSS</t>
         </is>
       </c>
-      <c r="T10" t="n">
+      <c r="T10" s="5" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="U10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>2026-01-11</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="5" t="n">
         <v>2025020715</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="C11" s="7" t="n"/>
+      <c r="D11" s="6" t="n"/>
+      <c r="E11" s="5" t="n"/>
+      <c r="F11" s="5" t="n"/>
+      <c r="G11" s="5" t="n"/>
+      <c r="H11" s="7" t="inlineStr">
         <is>
           <t>VGK</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" s="7" t="inlineStr">
         <is>
           <t>SJS</t>
         </is>
       </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="inlineStr">
+      <c r="J11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6" t="n"/>
+      <c r="L11" s="6" t="n"/>
+      <c r="M11" s="6" t="n"/>
+      <c r="N11" s="7" t="n"/>
+      <c r="O11" s="7" t="n"/>
+      <c r="P11" s="5" t="n"/>
+      <c r="Q11" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
+      <c r="R11" s="5" t="n"/>
+      <c r="S11" s="7" t="n"/>
+      <c r="T11" s="5" t="n"/>
+      <c r="U11" s="7" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4429,25 +4964,25 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="16" max="16"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="17" max="17"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="18" max="18"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="19" max="19"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="20" max="20"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="20" max="20"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="21" max="21"/>
   </cols>
   <sheetData>
@@ -6546,25 +7081,25 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="16" max="16"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="17" max="17"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="18" max="18"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="19" max="19"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="20" max="20"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="20" max="20"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="21" max="21"/>
   </cols>
   <sheetData>
@@ -7151,25 +7686,25 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="16" max="16"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="17" max="17"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="18" max="18"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="19" max="19"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="20" max="20"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="20" max="20"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="21" max="21"/>
   </cols>
   <sheetData>
@@ -8976,23 +9511,23 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="16" max="16"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="17" max="17"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="18" max="18"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="19" max="19"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="20" max="20"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="21" max="21"/>
@@ -9867,25 +10402,25 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="16" max="16"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="17" max="17"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="18" max="18"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="19" max="19"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="20" max="20"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="20" max="20"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="21" max="21"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
feat: add feature order back
</commit_message>
<xml_diff>
--- a/betting_tracker.xlsx
+++ b/betting_tracker.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,19 +27,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFffffff"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="14"/>
     </font>
     <font>
-      <b val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="12"/>
     </font>
     <font>
       <b val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
     </font>
   </fonts>
   <fills count="3">
@@ -52,12 +69,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="004472C4"/>
-        <bgColor rgb="004472C4"/>
+        <fgColor rgb="FF4472c4"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -65,21 +81,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -158,10 +238,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -199,69 +279,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -285,54 +367,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -342,7 +423,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -351,7 +432,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -360,7 +441,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -368,10 +449,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -400,7 +481,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -413,13 +494,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -439,7 +519,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:E23"/>
@@ -449,248 +529,323 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="5" max="5"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>BETTING PERFORMANCE SUMMARY</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="E1" s="10" t="n"/>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="7" t="n"/>
+      <c r="B2" s="10" t="n"/>
+      <c r="C2" s="10" t="n"/>
+      <c r="D2" s="10" t="n"/>
+      <c r="E2" s="10" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Generated:</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="10" t="inlineStr">
         <is>
           <t>2026-01-13 09:22:22</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="C3" s="10" t="n"/>
+      <c r="D3" s="10" t="n"/>
+      <c r="E3" s="10" t="n"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="7" t="n"/>
+      <c r="B4" s="10" t="n"/>
+      <c r="C4" s="10" t="n"/>
+      <c r="D4" s="10" t="n"/>
+      <c r="E4" s="10" t="n"/>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="13" t="inlineStr">
         <is>
           <t>OVERALL PERFORMANCE</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="B5" s="10" t="n"/>
+      <c r="C5" s="10" t="n"/>
+      <c r="D5" s="10" t="n"/>
+      <c r="E5" s="10" t="n"/>
+    </row>
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="7" t="n"/>
+      <c r="B6" s="10" t="n"/>
+      <c r="C6" s="10" t="n"/>
+      <c r="D6" s="10" t="n"/>
+      <c r="E6" s="10" t="n"/>
+    </row>
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>Total Bets</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="B7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10" t="n"/>
+      <c r="D7" s="10" t="n"/>
+      <c r="E7" s="10" t="n"/>
+    </row>
+    <row r="8" ht="18.75" customHeight="1">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="B8" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10" t="n"/>
+      <c r="D8" s="10" t="n"/>
+      <c r="E8" s="10" t="n"/>
+    </row>
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="B9" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10" t="n"/>
+      <c r="D9" s="10" t="n"/>
+      <c r="E9" s="10" t="n"/>
+    </row>
+    <row r="10" ht="18.75" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>Pushes</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="B10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10" t="n"/>
+      <c r="D10" s="10" t="n"/>
+      <c r="E10" s="10" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Win Rate</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="B11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10" t="n"/>
+      <c r="D11" s="10" t="n"/>
+      <c r="E11" s="10" t="n"/>
+    </row>
+    <row r="12" ht="18.75" customHeight="1">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>Total Profit/Loss</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="B12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10" t="n"/>
+      <c r="D12" s="10" t="n"/>
+      <c r="E12" s="10" t="n"/>
+    </row>
+    <row r="13" ht="18.75" customHeight="1">
+      <c r="A13" s="7" t="inlineStr">
         <is>
           <t>ROI %</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
+      <c r="B13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10" t="n"/>
+      <c r="D13" s="10" t="n"/>
+      <c r="E13" s="10" t="n"/>
+    </row>
+    <row r="14" ht="18.75" customHeight="1">
+      <c r="A14" s="7" t="n"/>
+      <c r="B14" s="10" t="n"/>
+      <c r="C14" s="10" t="n"/>
+      <c r="D14" s="10" t="n"/>
+      <c r="E14" s="10" t="n"/>
+    </row>
+    <row r="15" ht="18.75" customHeight="1">
+      <c r="A15" s="7" t="n"/>
+      <c r="B15" s="10" t="n"/>
+      <c r="C15" s="10" t="n"/>
+      <c r="D15" s="10" t="n"/>
+      <c r="E15" s="10" t="n"/>
+    </row>
+    <row r="16" ht="18.75" customHeight="1">
+      <c r="A16" s="13" t="inlineStr">
         <is>
           <t>PERFORMANCE BY CONFIDENCE LEVEL</t>
         </is>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="inlineStr">
+      <c r="B16" s="10" t="n"/>
+      <c r="C16" s="10" t="n"/>
+      <c r="D16" s="10" t="n"/>
+      <c r="E16" s="10" t="n"/>
+    </row>
+    <row r="17" ht="18.75" customHeight="1">
+      <c r="A17" s="11" t="inlineStr">
         <is>
           <t>Confidence</t>
         </is>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B17" s="12" t="inlineStr">
         <is>
           <t>Bets</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
+      <c r="C17" s="12" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr">
+      <c r="D17" s="12" t="inlineStr">
         <is>
           <t>Win Rate</t>
         </is>
       </c>
-      <c r="E17" s="3" t="inlineStr">
+      <c r="E17" s="12" t="inlineStr">
         <is>
           <t>ROI %</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="18" ht="18.75" customHeight="1">
+      <c r="A18" s="7" t="inlineStr">
         <is>
           <t>50-55%</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="B18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75" customHeight="1">
+      <c r="A19" s="7" t="inlineStr">
         <is>
           <t>55-60%</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="B19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" ht="18.75" customHeight="1">
+      <c r="A20" s="7" t="inlineStr">
         <is>
           <t>60-65%</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="B20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" ht="18.75" customHeight="1">
+      <c r="A21" s="7" t="inlineStr">
         <is>
           <t>65-70%</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="B21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" ht="18.75" customHeight="1">
+      <c r="A22" s="7" t="inlineStr">
         <is>
           <t>70-75%</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="B22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" ht="18.75" customHeight="1">
+      <c r="A23" s="7" t="inlineStr">
         <is>
           <t>75%+</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="n">
+      <c r="B23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -698,14 +853,14 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B13"/>
@@ -716,115 +871,128 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="30.005" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
+    <col width="20.005" bestFit="1" customWidth="1" style="10" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>BETTING TRACKER SETTINGS</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="B1" s="10" t="n"/>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="7" t="n"/>
+      <c r="B2" s="10" t="n"/>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>Setting</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="12" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>Default Unit Size</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Min Confidence to Bet (%)</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="4" t="n">
         <v>55</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>High Confidence Threshold (%)</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="4" t="n">
         <v>65</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>Min Expected Value (%)</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="4" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="8" ht="18.75" customHeight="1">
+      <c r="A8" s="7" t="n"/>
+      <c r="B8" s="10" t="n"/>
+    </row>
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>Odds Format</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="10" t="inlineStr">
         <is>
           <t>American</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="10" ht="18.75" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>Default Odds (if missing)</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="4" t="n">
         <v>-110</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="11" ht="18.75" customHeight="1">
+      <c r="A11" s="7" t="n"/>
+      <c r="B11" s="10" t="n"/>
+    </row>
+    <row r="12" ht="18.75" customHeight="1">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>Model Path</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="10" t="inlineStr">
         <is>
           <t>models/classifier_model.json</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="13" ht="18.75" customHeight="1">
+      <c r="A13" s="7" t="inlineStr">
         <is>
           <t>Feature Count</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="4" t="n">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -837,137 +1005,113 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="18" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="14" customWidth="1" min="13" max="13"/>
-    <col width="16" customWidth="1" min="14" max="14"/>
-    <col width="15" customWidth="1" min="15" max="15"/>
-    <col width="12" customWidth="1" min="16" max="16"/>
-    <col width="14" customWidth="1" min="17" max="17"/>
-    <col width="13" customWidth="1" min="18" max="18"/>
-    <col width="10" customWidth="1" min="19" max="19"/>
-    <col width="12" customWidth="1" min="20" max="20"/>
-    <col width="30" customWidth="1" min="21" max="21"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="14" t="inlineStr">
         <is>
           <t>game_date</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="14" t="inlineStr">
         <is>
           <t>game_id</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="14" t="inlineStr">
         <is>
           <t>goalie_name</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="14" t="inlineStr">
         <is>
           <t>betting_line</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="14" t="inlineStr">
         <is>
           <t>line_over</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="14" t="inlineStr">
         <is>
           <t>line_under</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="14" t="inlineStr">
         <is>
           <t>goalie_id</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="14" t="inlineStr">
         <is>
           <t>team_abbrev</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="14" t="inlineStr">
         <is>
           <t>opponent_team</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="J1" s="14" t="inlineStr">
         <is>
           <t>is_home</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="K1" s="14" t="inlineStr">
         <is>
           <t>predicted_saves</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="L1" s="14" t="inlineStr">
         <is>
           <t>prob_over</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="M1" s="14" t="inlineStr">
         <is>
           <t>confidence_pct</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="N1" s="14" t="inlineStr">
         <is>
           <t>confidence_bucket</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="O1" s="14" t="inlineStr">
         <is>
           <t>recommendation</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="P1" s="14" t="inlineStr">
         <is>
           <t>bet_amount</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="Q1" s="14" t="inlineStr">
         <is>
           <t>bet_selection</t>
         </is>
       </c>
-      <c r="R1" s="4" t="inlineStr">
+      <c r="R1" s="14" t="inlineStr">
         <is>
           <t>actual_saves</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
+      <c r="S1" s="14" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="T1" s="4" t="inlineStr">
+      <c r="T1" s="14" t="inlineStr">
         <is>
           <t>profit_loss</t>
         </is>
       </c>
-      <c r="U1" s="4" t="inlineStr">
+      <c r="U1" s="14" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
@@ -982,10 +1126,23 @@
       <c r="B2" t="n">
         <v>2025020725</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>meriläinen</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-115</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-113</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8482447</v>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>OTT</t>
@@ -999,11 +1156,25 @@
       <c r="J2" t="n">
         <v>1</v>
       </c>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>21.60000038146973</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.5157480239868164</v>
+      </c>
+      <c r="M2" t="n">
+        <v>3.149604797363281</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
@@ -1028,6 +1199,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>VAN</t>
@@ -1066,10 +1238,23 @@
       <c r="B4" t="n">
         <v>2025020726</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>silovs</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-109</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-120</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8481668</v>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
           <t>PIT</t>
@@ -1083,11 +1268,25 @@
       <c r="J4" t="n">
         <v>1</v>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>22.70000076293945</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.5427504777908325</v>
+      </c>
+      <c r="M4" t="n">
+        <v>8.550095558166504</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
@@ -1112,6 +1311,7 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
           <t>TBL</t>
@@ -1150,10 +1350,23 @@
       <c r="B6" t="n">
         <v>2025020727</v>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>thompson</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-117</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-112</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8480313</v>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>WSH</t>
@@ -1167,11 +1380,25 @@
       <c r="J6" t="n">
         <v>1</v>
       </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+      <c r="K6" t="n">
+        <v>22.70000076293945</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5308555960655212</v>
+      </c>
+      <c r="M6" t="n">
+        <v>6.171119213104248</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
@@ -1196,6 +1423,7 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>MTL</t>
@@ -1234,10 +1462,23 @@
       <c r="B8" t="n">
         <v>2025020728</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>greaves</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-108</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-121</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8482982</v>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
           <t>CBJ</t>
@@ -1251,11 +1492,25 @@
       <c r="J8" t="n">
         <v>1</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>26.60000038146973</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.510789155960083</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2.157831192016602</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
@@ -1276,10 +1531,23 @@
       <c r="B9" t="n">
         <v>2025020728</v>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>wolf</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-104</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-120</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8481692</v>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>CGY</t>
@@ -1293,11 +1561,25 @@
       <c r="J9" t="n">
         <v>0</v>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+      <c r="K9" t="n">
+        <v>26.39999961853027</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.4872313737869263</v>
+      </c>
+      <c r="M9" t="n">
+        <v>2.553725242614746</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
@@ -1318,10 +1600,23 @@
       <c r="B10" t="n">
         <v>2025020729</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>swayman</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-114</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-108</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8480280</v>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
           <t>BOS</t>
@@ -1335,11 +1630,25 @@
       <c r="J10" t="n">
         <v>1</v>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>23.60000038146973</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.5218905210494995</v>
+      </c>
+      <c r="M10" t="n">
+        <v>4.378104209899902</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
@@ -1364,6 +1673,7 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>DET</t>
@@ -1402,10 +1712,23 @@
       <c r="B12" t="n">
         <v>2025020730</v>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>hofer</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-115</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-107</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8480981</v>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
           <t>STL</t>
@@ -1419,11 +1742,25 @@
       <c r="J12" t="n">
         <v>1</v>
       </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="K12" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.4923161268234253</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1.536774635314941</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
@@ -1448,6 +1785,7 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>CAR</t>
@@ -1486,10 +1824,23 @@
       <c r="B14" t="n">
         <v>2025020731</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>saros</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-103</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8477424</v>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
           <t>NSH</t>
@@ -1503,11 +1854,25 @@
       <c r="J14" t="n">
         <v>1</v>
       </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>24.60000038146973</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.5277358889579773</v>
+      </c>
+      <c r="M14" t="n">
+        <v>5.547177791595459</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
@@ -1532,6 +1897,7 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>EDM</t>
@@ -1574,6 +1940,7 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>WPG</t>
@@ -1616,6 +1983,7 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>NYI</t>
@@ -1658,6 +2026,7 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
           <t>UTA</t>
@@ -1700,6 +2069,7 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
           <t>TOR</t>
@@ -1742,6 +2112,7 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
           <t>ANA</t>
@@ -1784,6 +2155,7 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
           <t>DAL</t>

</xml_diff>

<commit_message>
feat: switched to a better model
</commit_message>
<xml_diff>
--- a/betting_tracker.xlsx
+++ b/betting_tracker.xlsx
@@ -29,7 +29,7 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FFffffff"/>
+      <color theme="1"/>
       <sz val="11"/>
     </font>
     <font>
@@ -41,36 +41,31 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="14"/>
     </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="12"/>
     </font>
     <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4472c4"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -83,16 +78,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -113,12 +108,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -126,6 +124,12 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
@@ -139,10 +143,16 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -150,6 +160,9 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -530,322 +543,322 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="10" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="18" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="18" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="18" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="18" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="14" t="inlineStr">
         <is>
           <t>BETTING PERFORMANCE SUMMARY</t>
         </is>
       </c>
-      <c r="E1" s="10" t="n"/>
+      <c r="E1" s="15" t="n"/>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="7" t="n"/>
-      <c r="B2" s="10" t="n"/>
-      <c r="C2" s="10" t="n"/>
-      <c r="D2" s="10" t="n"/>
-      <c r="E2" s="10" t="n"/>
+      <c r="A2" s="10" t="n"/>
+      <c r="B2" s="15" t="n"/>
+      <c r="C2" s="15" t="n"/>
+      <c r="D2" s="15" t="n"/>
+      <c r="E2" s="15" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="10" t="inlineStr">
         <is>
           <t>Generated:</t>
         </is>
       </c>
-      <c r="B3" s="10" t="inlineStr">
+      <c r="B3" s="15" t="inlineStr">
         <is>
           <t>2026-01-13 09:22:22</t>
         </is>
       </c>
-      <c r="C3" s="10" t="n"/>
-      <c r="D3" s="10" t="n"/>
-      <c r="E3" s="10" t="n"/>
+      <c r="C3" s="15" t="n"/>
+      <c r="D3" s="15" t="n"/>
+      <c r="E3" s="15" t="n"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="7" t="n"/>
-      <c r="B4" s="10" t="n"/>
-      <c r="C4" s="10" t="n"/>
-      <c r="D4" s="10" t="n"/>
-      <c r="E4" s="10" t="n"/>
+      <c r="A4" s="10" t="n"/>
+      <c r="B4" s="15" t="n"/>
+      <c r="C4" s="15" t="n"/>
+      <c r="D4" s="15" t="n"/>
+      <c r="E4" s="15" t="n"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="13" t="inlineStr">
+      <c r="A5" s="19" t="inlineStr">
         <is>
           <t>OVERALL PERFORMANCE</t>
         </is>
       </c>
-      <c r="B5" s="10" t="n"/>
-      <c r="C5" s="10" t="n"/>
-      <c r="D5" s="10" t="n"/>
-      <c r="E5" s="10" t="n"/>
+      <c r="B5" s="15" t="n"/>
+      <c r="C5" s="15" t="n"/>
+      <c r="D5" s="15" t="n"/>
+      <c r="E5" s="15" t="n"/>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="7" t="n"/>
-      <c r="B6" s="10" t="n"/>
-      <c r="C6" s="10" t="n"/>
-      <c r="D6" s="10" t="n"/>
-      <c r="E6" s="10" t="n"/>
+      <c r="A6" s="10" t="n"/>
+      <c r="B6" s="15" t="n"/>
+      <c r="C6" s="15" t="n"/>
+      <c r="D6" s="15" t="n"/>
+      <c r="E6" s="15" t="n"/>
     </row>
     <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>Total Bets</t>
         </is>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="10" t="n"/>
-      <c r="D7" s="10" t="n"/>
-      <c r="E7" s="10" t="n"/>
+      <c r="B7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15" t="n"/>
+      <c r="D7" s="15" t="n"/>
+      <c r="E7" s="15" t="n"/>
     </row>
     <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="7" t="inlineStr">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="10" t="n"/>
-      <c r="D8" s="10" t="n"/>
-      <c r="E8" s="10" t="n"/>
+      <c r="B8" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="15" t="n"/>
+      <c r="D8" s="15" t="n"/>
+      <c r="E8" s="15" t="n"/>
     </row>
     <row r="9" ht="18.75" customHeight="1">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="10" t="inlineStr">
         <is>
           <t>Losses</t>
         </is>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="10" t="n"/>
-      <c r="D9" s="10" t="n"/>
-      <c r="E9" s="10" t="n"/>
+      <c r="B9" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="15" t="n"/>
+      <c r="D9" s="15" t="n"/>
+      <c r="E9" s="15" t="n"/>
     </row>
     <row r="10" ht="18.75" customHeight="1">
-      <c r="A10" s="7" t="inlineStr">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>Pushes</t>
         </is>
       </c>
-      <c r="B10" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="10" t="n"/>
-      <c r="D10" s="10" t="n"/>
-      <c r="E10" s="10" t="n"/>
+      <c r="B10" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="15" t="n"/>
+      <c r="D10" s="15" t="n"/>
+      <c r="E10" s="15" t="n"/>
     </row>
     <row r="11" ht="18.75" customHeight="1">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>Win Rate</t>
         </is>
       </c>
-      <c r="B11" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="10" t="n"/>
-      <c r="D11" s="10" t="n"/>
-      <c r="E11" s="10" t="n"/>
+      <c r="B11" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15" t="n"/>
+      <c r="D11" s="15" t="n"/>
+      <c r="E11" s="15" t="n"/>
     </row>
     <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="7" t="inlineStr">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>Total Profit/Loss</t>
         </is>
       </c>
-      <c r="B12" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="10" t="n"/>
-      <c r="D12" s="10" t="n"/>
-      <c r="E12" s="10" t="n"/>
+      <c r="B12" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="15" t="n"/>
+      <c r="D12" s="15" t="n"/>
+      <c r="E12" s="15" t="n"/>
     </row>
     <row r="13" ht="18.75" customHeight="1">
-      <c r="A13" s="7" t="inlineStr">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <t>ROI %</t>
         </is>
       </c>
-      <c r="B13" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="10" t="n"/>
-      <c r="D13" s="10" t="n"/>
-      <c r="E13" s="10" t="n"/>
+      <c r="B13" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="15" t="n"/>
+      <c r="D13" s="15" t="n"/>
+      <c r="E13" s="15" t="n"/>
     </row>
     <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="7" t="n"/>
-      <c r="B14" s="10" t="n"/>
-      <c r="C14" s="10" t="n"/>
-      <c r="D14" s="10" t="n"/>
-      <c r="E14" s="10" t="n"/>
+      <c r="A14" s="10" t="n"/>
+      <c r="B14" s="15" t="n"/>
+      <c r="C14" s="15" t="n"/>
+      <c r="D14" s="15" t="n"/>
+      <c r="E14" s="15" t="n"/>
     </row>
     <row r="15" ht="18.75" customHeight="1">
-      <c r="A15" s="7" t="n"/>
-      <c r="B15" s="10" t="n"/>
-      <c r="C15" s="10" t="n"/>
-      <c r="D15" s="10" t="n"/>
-      <c r="E15" s="10" t="n"/>
+      <c r="A15" s="10" t="n"/>
+      <c r="B15" s="15" t="n"/>
+      <c r="C15" s="15" t="n"/>
+      <c r="D15" s="15" t="n"/>
+      <c r="E15" s="15" t="n"/>
     </row>
     <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="13" t="inlineStr">
+      <c r="A16" s="19" t="inlineStr">
         <is>
           <t>PERFORMANCE BY CONFIDENCE LEVEL</t>
         </is>
       </c>
-      <c r="B16" s="10" t="n"/>
-      <c r="C16" s="10" t="n"/>
-      <c r="D16" s="10" t="n"/>
-      <c r="E16" s="10" t="n"/>
+      <c r="B16" s="15" t="n"/>
+      <c r="C16" s="15" t="n"/>
+      <c r="D16" s="15" t="n"/>
+      <c r="E16" s="15" t="n"/>
     </row>
     <row r="17" ht="18.75" customHeight="1">
-      <c r="A17" s="11" t="inlineStr">
+      <c r="A17" s="16" t="inlineStr">
         <is>
           <t>Confidence</t>
         </is>
       </c>
-      <c r="B17" s="12" t="inlineStr">
+      <c r="B17" s="17" t="inlineStr">
         <is>
           <t>Bets</t>
         </is>
       </c>
-      <c r="C17" s="12" t="inlineStr">
+      <c r="C17" s="17" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="D17" s="12" t="inlineStr">
+      <c r="D17" s="17" t="inlineStr">
         <is>
           <t>Win Rate</t>
         </is>
       </c>
-      <c r="E17" s="12" t="inlineStr">
+      <c r="E17" s="17" t="inlineStr">
         <is>
           <t>ROI %</t>
         </is>
       </c>
     </row>
     <row r="18" ht="18.75" customHeight="1">
-      <c r="A18" s="7" t="inlineStr">
+      <c r="A18" s="10" t="inlineStr">
         <is>
           <t>50-55%</t>
         </is>
       </c>
-      <c r="B18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4" t="n">
+      <c r="B18" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" ht="18.75" customHeight="1">
-      <c r="A19" s="7" t="inlineStr">
+      <c r="A19" s="10" t="inlineStr">
         <is>
           <t>55-60%</t>
         </is>
       </c>
-      <c r="B19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4" t="n">
+      <c r="B19" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" ht="18.75" customHeight="1">
-      <c r="A20" s="7" t="inlineStr">
+      <c r="A20" s="10" t="inlineStr">
         <is>
           <t>60-65%</t>
         </is>
       </c>
-      <c r="B20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4" t="n">
+      <c r="B20" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" ht="18.75" customHeight="1">
-      <c r="A21" s="7" t="inlineStr">
+      <c r="A21" s="10" t="inlineStr">
         <is>
           <t>65-70%</t>
         </is>
       </c>
-      <c r="B21" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="4" t="n">
+      <c r="B21" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="7" t="inlineStr">
+      <c r="A22" s="10" t="inlineStr">
         <is>
           <t>70-75%</t>
         </is>
       </c>
-      <c r="B22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="4" t="n">
+      <c r="B22" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" ht="18.75" customHeight="1">
-      <c r="A23" s="7" t="inlineStr">
+      <c r="A23" s="10" t="inlineStr">
         <is>
           <t>75%+</t>
         </is>
       </c>
-      <c r="B23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4" t="n">
+      <c r="B23" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -871,123 +884,123 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30.005" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="20.005" bestFit="1" customWidth="1" style="10" min="2" max="2"/>
+    <col width="30.005" bestFit="1" customWidth="1" style="10" min="1" max="1"/>
+    <col width="20.005" bestFit="1" customWidth="1" style="18" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="9" t="inlineStr">
+      <c r="A1" s="14" t="inlineStr">
         <is>
           <t>BETTING TRACKER SETTINGS</t>
         </is>
       </c>
-      <c r="B1" s="10" t="n"/>
+      <c r="B1" s="15" t="n"/>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="7" t="n"/>
-      <c r="B2" s="10" t="n"/>
+      <c r="A2" s="10" t="n"/>
+      <c r="B2" s="15" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="11" t="inlineStr">
+      <c r="A3" s="16" t="inlineStr">
         <is>
           <t>Setting</t>
         </is>
       </c>
-      <c r="B3" s="12" t="inlineStr">
+      <c r="B3" s="17" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="7" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>Default Unit Size</t>
         </is>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="15" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
         <is>
           <t>Min Confidence to Bet (%)</t>
         </is>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="15" t="n">
         <v>55</v>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="7" t="inlineStr">
+      <c r="A6" s="10" t="inlineStr">
         <is>
           <t>High Confidence Threshold (%)</t>
         </is>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="15" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="A7" s="10" t="inlineStr">
         <is>
           <t>Min Expected Value (%)</t>
         </is>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="15" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="7" t="n"/>
-      <c r="B8" s="10" t="n"/>
+      <c r="A8" s="10" t="n"/>
+      <c r="B8" s="15" t="n"/>
     </row>
     <row r="9" ht="18.75" customHeight="1">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="10" t="inlineStr">
         <is>
           <t>Odds Format</t>
         </is>
       </c>
-      <c r="B9" s="10" t="inlineStr">
+      <c r="B9" s="15" t="inlineStr">
         <is>
           <t>American</t>
         </is>
       </c>
     </row>
     <row r="10" ht="18.75" customHeight="1">
-      <c r="A10" s="7" t="inlineStr">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>Default Odds (if missing)</t>
         </is>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="15" t="n">
         <v>-110</v>
       </c>
     </row>
     <row r="11" ht="18.75" customHeight="1">
-      <c r="A11" s="7" t="n"/>
-      <c r="B11" s="10" t="n"/>
+      <c r="A11" s="10" t="n"/>
+      <c r="B11" s="15" t="n"/>
     </row>
     <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="7" t="inlineStr">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>Model Path</t>
         </is>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="15" t="inlineStr">
         <is>
           <t>models/classifier_model.json</t>
         </is>
       </c>
     </row>
     <row r="13" ht="18.75" customHeight="1">
-      <c r="A13" s="7" t="inlineStr">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <t>Feature Count</t>
         </is>
       </c>
-      <c r="B13" s="4" t="n">
+      <c r="B13" s="15" t="n">
         <v>89</v>
       </c>
     </row>
@@ -1011,107 +1024,107 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="inlineStr">
+      <c r="A1" s="20" t="inlineStr">
         <is>
           <t>game_date</t>
         </is>
       </c>
-      <c r="B1" s="14" t="inlineStr">
+      <c r="B1" s="20" t="inlineStr">
         <is>
           <t>game_id</t>
         </is>
       </c>
-      <c r="C1" s="14" t="inlineStr">
+      <c r="C1" s="20" t="inlineStr">
         <is>
           <t>goalie_name</t>
         </is>
       </c>
-      <c r="D1" s="14" t="inlineStr">
+      <c r="D1" s="20" t="inlineStr">
         <is>
           <t>betting_line</t>
         </is>
       </c>
-      <c r="E1" s="14" t="inlineStr">
+      <c r="E1" s="20" t="inlineStr">
         <is>
           <t>line_over</t>
         </is>
       </c>
-      <c r="F1" s="14" t="inlineStr">
+      <c r="F1" s="20" t="inlineStr">
         <is>
           <t>line_under</t>
         </is>
       </c>
-      <c r="G1" s="14" t="inlineStr">
+      <c r="G1" s="20" t="inlineStr">
         <is>
           <t>goalie_id</t>
         </is>
       </c>
-      <c r="H1" s="14" t="inlineStr">
+      <c r="H1" s="20" t="inlineStr">
         <is>
           <t>team_abbrev</t>
         </is>
       </c>
-      <c r="I1" s="14" t="inlineStr">
+      <c r="I1" s="20" t="inlineStr">
         <is>
           <t>opponent_team</t>
         </is>
       </c>
-      <c r="J1" s="14" t="inlineStr">
+      <c r="J1" s="20" t="inlineStr">
         <is>
           <t>is_home</t>
         </is>
       </c>
-      <c r="K1" s="14" t="inlineStr">
+      <c r="K1" s="20" t="inlineStr">
         <is>
           <t>predicted_saves</t>
         </is>
       </c>
-      <c r="L1" s="14" t="inlineStr">
+      <c r="L1" s="20" t="inlineStr">
         <is>
           <t>prob_over</t>
         </is>
       </c>
-      <c r="M1" s="14" t="inlineStr">
+      <c r="M1" s="20" t="inlineStr">
         <is>
           <t>confidence_pct</t>
         </is>
       </c>
-      <c r="N1" s="14" t="inlineStr">
+      <c r="N1" s="20" t="inlineStr">
         <is>
           <t>confidence_bucket</t>
         </is>
       </c>
-      <c r="O1" s="14" t="inlineStr">
+      <c r="O1" s="20" t="inlineStr">
         <is>
           <t>recommendation</t>
         </is>
       </c>
-      <c r="P1" s="14" t="inlineStr">
+      <c r="P1" s="20" t="inlineStr">
         <is>
           <t>bet_amount</t>
         </is>
       </c>
-      <c r="Q1" s="14" t="inlineStr">
+      <c r="Q1" s="20" t="inlineStr">
         <is>
           <t>bet_selection</t>
         </is>
       </c>
-      <c r="R1" s="14" t="inlineStr">
+      <c r="R1" s="20" t="inlineStr">
         <is>
           <t>actual_saves</t>
         </is>
       </c>
-      <c r="S1" s="14" t="inlineStr">
+      <c r="S1" s="20" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="T1" s="14" t="inlineStr">
+      <c r="T1" s="20" t="inlineStr">
         <is>
           <t>profit_loss</t>
         </is>
       </c>
-      <c r="U1" s="14" t="inlineStr">
+      <c r="U1" s="20" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
@@ -1135,10 +1148,10 @@
         <v>21.5</v>
       </c>
       <c r="E2" t="n">
+        <v>-113</v>
+      </c>
+      <c r="F2" t="n">
         <v>-115</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-113</v>
       </c>
       <c r="G2" t="n">
         <v>8482447</v>
@@ -1160,10 +1173,10 @@
         <v>21.60000038146973</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5157480239868164</v>
+        <v>0.5126954913139343</v>
       </c>
       <c r="M2" t="n">
-        <v>3.149604797363281</v>
+        <v>2.539098262786865</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -1195,11 +1208,23 @@
       <c r="B3" t="n">
         <v>2025020725</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>lankinen</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-118</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-110</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8480947</v>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>VAN</t>
@@ -1213,11 +1238,25 @@
       <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.4920174479484558</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1.596510410308838</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
@@ -1247,10 +1286,10 @@
         <v>22.5</v>
       </c>
       <c r="E4" t="n">
-        <v>-109</v>
+        <v>-112</v>
       </c>
       <c r="F4" t="n">
-        <v>-120</v>
+        <v>-117</v>
       </c>
       <c r="G4" t="n">
         <v>8481668</v>
@@ -1272,10 +1311,10 @@
         <v>22.70000076293945</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5427504777908325</v>
+        <v>0.5380865335464478</v>
       </c>
       <c r="M4" t="n">
-        <v>8.550095558166504</v>
+        <v>7.617306709289551</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -1307,11 +1346,23 @@
       <c r="B5" t="n">
         <v>2025020726</v>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>vasilevskiy</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-113</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-115</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8476883</v>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
           <t>TBL</t>
@@ -1325,11 +1376,25 @@
       <c r="J5" t="n">
         <v>0</v>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>24.60000038146973</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.5146847367286682</v>
+      </c>
+      <c r="M5" t="n">
+        <v>2.936947345733643</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
@@ -1359,10 +1424,10 @@
         <v>22.5</v>
       </c>
       <c r="E6" t="n">
-        <v>-117</v>
+        <v>-124</v>
       </c>
       <c r="F6" t="n">
-        <v>-112</v>
+        <v>-106</v>
       </c>
       <c r="G6" t="n">
         <v>8480313</v>
@@ -1381,13 +1446,13 @@
         <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>22.70000076293945</v>
+        <v>22.60000038146973</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5308555960655212</v>
+        <v>0.5291582345962524</v>
       </c>
       <c r="M6" t="n">
-        <v>6.171119213104248</v>
+        <v>5.831646919250488</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1419,11 +1484,23 @@
       <c r="B7" t="n">
         <v>2025020727</v>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>montembeault</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-125</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-104</v>
+      </c>
+      <c r="G7" t="n">
+        <v>8478470</v>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
           <t>MTL</t>
@@ -1437,11 +1514,25 @@
       <c r="J7" t="n">
         <v>0</v>
       </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
+      <c r="K7" t="n">
+        <v>23.60000038146973</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.5148718357086182</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2.974367141723633</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
@@ -1471,10 +1562,10 @@
         <v>26.5</v>
       </c>
       <c r="E8" t="n">
-        <v>-108</v>
+        <v>-107</v>
       </c>
       <c r="F8" t="n">
-        <v>-121</v>
+        <v>-122</v>
       </c>
       <c r="G8" t="n">
         <v>8482982</v>
@@ -1496,10 +1587,10 @@
         <v>26.60000038146973</v>
       </c>
       <c r="L8" t="n">
-        <v>0.510789155960083</v>
+        <v>0.5237208008766174</v>
       </c>
       <c r="M8" t="n">
-        <v>2.157831192016602</v>
+        <v>4.744160175323486</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1540,10 +1631,10 @@
         <v>26.5</v>
       </c>
       <c r="E9" t="n">
-        <v>-104</v>
+        <v>-103</v>
       </c>
       <c r="F9" t="n">
-        <v>-120</v>
+        <v>-127</v>
       </c>
       <c r="G9" t="n">
         <v>8481692</v>
@@ -1565,10 +1656,10 @@
         <v>26.39999961853027</v>
       </c>
       <c r="L9" t="n">
-        <v>0.4872313737869263</v>
+        <v>0.4788225293159485</v>
       </c>
       <c r="M9" t="n">
-        <v>2.553725242614746</v>
+        <v>4.235494136810303</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1609,10 +1700,10 @@
         <v>23.5</v>
       </c>
       <c r="E10" t="n">
-        <v>-114</v>
+        <v>-118</v>
       </c>
       <c r="F10" t="n">
-        <v>-108</v>
+        <v>-110</v>
       </c>
       <c r="G10" t="n">
         <v>8480280</v>
@@ -1634,10 +1725,10 @@
         <v>23.60000038146973</v>
       </c>
       <c r="L10" t="n">
-        <v>0.5218905210494995</v>
+        <v>0.528777003288269</v>
       </c>
       <c r="M10" t="n">
-        <v>4.378104209899902</v>
+        <v>5.755400657653809</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1721,7 +1812,7 @@
         <v>26.5</v>
       </c>
       <c r="E12" t="n">
-        <v>-115</v>
+        <v>-122</v>
       </c>
       <c r="F12" t="n">
         <v>-107</v>
@@ -1746,10 +1837,10 @@
         <v>26.5</v>
       </c>
       <c r="L12" t="n">
-        <v>0.4923161268234253</v>
+        <v>0.4926919639110565</v>
       </c>
       <c r="M12" t="n">
-        <v>1.536774635314941</v>
+        <v>1.461607217788696</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1781,11 +1872,23 @@
       <c r="B13" t="n">
         <v>2025020730</v>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>bussi</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-118</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-105</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8483548</v>
+      </c>
       <c r="H13" t="inlineStr">
         <is>
           <t>CAR</t>
@@ -1799,11 +1902,25 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>19.79999923706055</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.553071916103363</v>
+      </c>
+      <c r="M13" t="n">
+        <v>10.61438369750977</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>55-60%</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
@@ -1833,10 +1950,10 @@
         <v>24.5</v>
       </c>
       <c r="E14" t="n">
-        <v>-120</v>
+        <v>-124</v>
       </c>
       <c r="F14" t="n">
-        <v>-103</v>
+        <v>-105</v>
       </c>
       <c r="G14" t="n">
         <v>8477424</v>
@@ -1855,13 +1972,13 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>24.60000038146973</v>
+        <v>24.70000076293945</v>
       </c>
       <c r="L14" t="n">
-        <v>0.5277358889579773</v>
+        <v>0.5351357460021973</v>
       </c>
       <c r="M14" t="n">
-        <v>5.547177791595459</v>
+        <v>7.027149200439453</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1936,11 +2053,23 @@
       <c r="B16" t="n">
         <v>2025020732</v>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>hellebuyck</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-130</v>
+      </c>
+      <c r="F16" t="n">
+        <v>100</v>
+      </c>
+      <c r="G16" t="n">
+        <v>8476945</v>
+      </c>
       <c r="H16" t="inlineStr">
         <is>
           <t>WPG</t>
@@ -1954,11 +2083,25 @@
       <c r="J16" t="n">
         <v>1</v>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+      <c r="K16" t="n">
+        <v>22.60000038146973</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.5217793583869934</v>
+      </c>
+      <c r="M16" t="n">
+        <v>4.355871677398682</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
@@ -1979,11 +2122,23 @@
       <c r="B17" t="n">
         <v>2025020732</v>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sorokin</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-129</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-102</v>
+      </c>
+      <c r="G17" t="n">
+        <v>8478009</v>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
           <t>NYI</t>
@@ -1997,11 +2152,25 @@
       <c r="J17" t="n">
         <v>0</v>
       </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+      <c r="K17" t="n">
+        <v>24.70000076293945</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.532870888710022</v>
+      </c>
+      <c r="M17" t="n">
+        <v>6.574177742004395</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr">
         <is>
@@ -2022,11 +2191,23 @@
       <c r="B18" t="n">
         <v>2025020733</v>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>vejmelka</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-129</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-102</v>
+      </c>
+      <c r="G18" t="n">
+        <v>8478872</v>
+      </c>
       <c r="H18" t="inlineStr">
         <is>
           <t>UTA</t>
@@ -2040,11 +2221,25 @@
       <c r="J18" t="n">
         <v>1</v>
       </c>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>21.60000038146973</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.5225210189819336</v>
+      </c>
+      <c r="M18" t="n">
+        <v>4.504203796386719</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr">
         <is>
@@ -2108,11 +2303,23 @@
       <c r="B20" t="n">
         <v>2025020734</v>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>dostal</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-124</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-105</v>
+      </c>
+      <c r="G20" t="n">
+        <v>8480843</v>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
           <t>ANA</t>
@@ -2126,11 +2333,25 @@
       <c r="J20" t="n">
         <v>1</v>
       </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
+      <c r="K20" t="n">
+        <v>22.79999923706055</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.5653749108314514</v>
+      </c>
+      <c r="M20" t="n">
+        <v>13.07498168945312</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>55-60%</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
feat: removed unnecessary scripts
</commit_message>
<xml_diff>
--- a/betting_tracker.xlsx
+++ b/betting_tracker.xlsx
@@ -125,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -154,23 +154,17 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
@@ -178,7 +172,16 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -582,14 +585,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="26" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="27" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="19" t="inlineStr">
+      <c r="A1" s="20" t="inlineStr">
         <is>
           <t>BETTING PERFORMANCE SUMMARY</t>
         </is>
@@ -626,7 +629,7 @@
       <c r="E4" s="5" t="n"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="24" t="inlineStr">
+      <c r="A5" s="25" t="inlineStr">
         <is>
           <t>OVERALL PERFORMANCE</t>
         </is>
@@ -755,7 +758,7 @@
       <c r="E15" s="5" t="n"/>
     </row>
     <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="24" t="inlineStr">
+      <c r="A16" s="25" t="inlineStr">
         <is>
           <t>PERFORMANCE BY CONFIDENCE LEVEL</t>
         </is>
@@ -766,27 +769,27 @@
       <c r="E16" s="5" t="n"/>
     </row>
     <row r="17" ht="18.75" customHeight="1">
-      <c r="A17" s="20" t="inlineStr">
+      <c r="A17" s="21" t="inlineStr">
         <is>
           <t>Confidence</t>
         </is>
       </c>
-      <c r="B17" s="21" t="inlineStr">
+      <c r="B17" s="22" t="inlineStr">
         <is>
           <t>Bets</t>
         </is>
       </c>
-      <c r="C17" s="21" t="inlineStr">
+      <c r="C17" s="22" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="D17" s="20" t="inlineStr">
+      <c r="D17" s="21" t="inlineStr">
         <is>
           <t>Win Rate</t>
         </is>
       </c>
-      <c r="E17" s="21" t="inlineStr">
+      <c r="E17" s="22" t="inlineStr">
         <is>
           <t>ROI %</t>
         </is>
@@ -804,7 +807,7 @@
       <c r="C18" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D18" s="25" t="inlineStr">
+      <c r="D18" s="26" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
@@ -827,7 +830,7 @@
       <c r="C19" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="D19" s="25" t="inlineStr">
+      <c r="D19" s="26" t="inlineStr">
         <is>
           <t>100.0%</t>
         </is>
@@ -850,7 +853,7 @@
       <c r="C20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="25" t="inlineStr">
+      <c r="D20" s="26" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
@@ -873,7 +876,7 @@
       <c r="C21" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D21" s="25" t="inlineStr">
+      <c r="D21" s="26" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
@@ -896,7 +899,7 @@
       <c r="C22" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D22" s="25" t="inlineStr">
+      <c r="D22" s="26" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
@@ -919,7 +922,7 @@
       <c r="C23" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="D23" s="25" t="inlineStr">
+      <c r="D23" s="26" t="inlineStr">
         <is>
           <t>0.0%</t>
         </is>
@@ -953,11 +956,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30.005" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="20.005" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
+    <col width="20.005" bestFit="1" customWidth="1" style="23" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="19" t="inlineStr">
+      <c r="A1" s="20" t="inlineStr">
         <is>
           <t>BETTING TRACKER SETTINGS</t>
         </is>
@@ -969,12 +972,12 @@
       <c r="B2" s="5" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="20" t="inlineStr">
+      <c r="A3" s="21" t="inlineStr">
         <is>
           <t>Setting</t>
         </is>
       </c>
-      <c r="B3" s="21" t="inlineStr">
+      <c r="B3" s="22" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
@@ -1092,112 +1095,112 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="27" t="inlineStr">
+      <c r="A1" s="28" t="inlineStr">
         <is>
           <t>game_date</t>
         </is>
       </c>
-      <c r="B1" s="27" t="inlineStr">
+      <c r="B1" s="28" t="inlineStr">
         <is>
           <t>game_id</t>
         </is>
       </c>
-      <c r="C1" s="27" t="inlineStr">
+      <c r="C1" s="28" t="inlineStr">
         <is>
           <t>goalie_name</t>
         </is>
       </c>
-      <c r="D1" s="27" t="inlineStr">
+      <c r="D1" s="28" t="inlineStr">
         <is>
           <t>betting_line</t>
         </is>
       </c>
-      <c r="E1" s="27" t="inlineStr">
+      <c r="E1" s="28" t="inlineStr">
         <is>
           <t>line_over</t>
         </is>
       </c>
-      <c r="F1" s="27" t="inlineStr">
+      <c r="F1" s="28" t="inlineStr">
         <is>
           <t>line_under</t>
         </is>
       </c>
-      <c r="G1" s="27" t="inlineStr">
+      <c r="G1" s="28" t="inlineStr">
         <is>
           <t>goalie_id</t>
         </is>
       </c>
-      <c r="H1" s="27" t="inlineStr">
+      <c r="H1" s="28" t="inlineStr">
         <is>
           <t>team_abbrev</t>
         </is>
       </c>
-      <c r="I1" s="27" t="inlineStr">
+      <c r="I1" s="28" t="inlineStr">
         <is>
           <t>opponent_team</t>
         </is>
       </c>
-      <c r="J1" s="27" t="inlineStr">
+      <c r="J1" s="28" t="inlineStr">
         <is>
           <t>is_home</t>
         </is>
       </c>
-      <c r="K1" s="27" t="inlineStr">
+      <c r="K1" s="28" t="inlineStr">
         <is>
           <t>predicted_saves</t>
         </is>
       </c>
-      <c r="L1" s="27" t="inlineStr">
+      <c r="L1" s="28" t="inlineStr">
         <is>
           <t>prob_over</t>
         </is>
       </c>
-      <c r="M1" s="27" t="inlineStr">
+      <c r="M1" s="28" t="inlineStr">
         <is>
           <t>confidence_pct</t>
         </is>
       </c>
-      <c r="N1" s="27" t="inlineStr">
+      <c r="N1" s="28" t="inlineStr">
         <is>
           <t>confidence_bucket</t>
         </is>
       </c>
-      <c r="O1" s="27" t="inlineStr">
+      <c r="O1" s="28" t="inlineStr">
         <is>
           <t>recommendation</t>
         </is>
       </c>
-      <c r="P1" s="27" t="inlineStr">
+      <c r="P1" s="28" t="inlineStr">
         <is>
           <t>ev</t>
         </is>
       </c>
-      <c r="Q1" s="27" t="inlineStr">
+      <c r="Q1" s="28" t="inlineStr">
         <is>
           <t>bet_amount</t>
         </is>
       </c>
-      <c r="R1" s="27" t="inlineStr">
+      <c r="R1" s="28" t="inlineStr">
         <is>
           <t>bet_selection</t>
         </is>
       </c>
-      <c r="S1" s="27" t="inlineStr">
+      <c r="S1" s="28" t="inlineStr">
         <is>
           <t>actual_saves</t>
         </is>
       </c>
-      <c r="T1" s="27" t="inlineStr">
+      <c r="T1" s="28" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="U1" s="27" t="inlineStr">
+      <c r="U1" s="28" t="inlineStr">
         <is>
           <t>profit_loss</t>
         </is>
       </c>
-      <c r="V1" s="27" t="inlineStr">
+      <c r="V1" s="28" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
@@ -1300,11 +1303,23 @@
       <c r="B4" t="n">
         <v>2025020741</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>skinner</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-115</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-106</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8479973</v>
+      </c>
       <c r="H4" t="inlineStr">
         <is>
           <t>PIT</t>
@@ -1318,12 +1333,28 @@
       <c r="J4" t="n">
         <v>1</v>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.5096580982208252</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1.931619644165039</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>-0.02422118186950684</v>
+      </c>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr">
         <is>
@@ -1422,10 +1453,10 @@
         <v>22.70000076293945</v>
       </c>
       <c r="L6" t="n">
-        <v>0.533284068107605</v>
+        <v>0.5344140529632568</v>
       </c>
       <c r="M6" t="n">
-        <v>6.656813621520996</v>
+        <v>6.882810592651367</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1438,7 +1469,7 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>0.0258948802947998</v>
+        <v>0.02702486515045166</v>
       </c>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr">
@@ -1491,13 +1522,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>26.5</v>
+        <v>26.39999961853027</v>
       </c>
       <c r="L7" t="n">
-        <v>0.4901469349861145</v>
+        <v>0.4711514115333557</v>
       </c>
       <c r="M7" t="n">
-        <v>1.9706130027771</v>
+        <v>5.769717693328857</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1510,7 +1541,7 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>-0.01395648717880249</v>
+        <v>0.005039036273956299</v>
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
@@ -1532,11 +1563,23 @@
       <c r="B8" t="n">
         <v>2025020743</v>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>merzlikins</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-112</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-110</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8478007</v>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
           <t>CBJ</t>
@@ -1550,12 +1593,28 @@
       <c r="J8" t="n">
         <v>1</v>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>23.60000038146973</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.5200234055519104</v>
+      </c>
+      <c r="M8" t="n">
+        <v>4.00468111038208</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>-0.008278489112854004</v>
+      </c>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
         <is>
@@ -1620,11 +1679,23 @@
       <c r="B10" t="n">
         <v>2025020739</v>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>swayman</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-115</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-107</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8480280</v>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
           <t>BOS</t>
@@ -1638,12 +1709,28 @@
       <c r="J10" t="n">
         <v>1</v>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>22.70000076293945</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.5357988476753235</v>
+      </c>
+      <c r="M10" t="n">
+        <v>7.159769535064697</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>0.0009151101112365723</v>
+      </c>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr">
         <is>
@@ -1796,11 +1883,21 @@
       <c r="B14" t="n">
         <v>2025020745</v>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>knight</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-107</v>
+      </c>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>8481519</v>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
           <t>CHI</t>
@@ -1814,12 +1911,28 @@
       <c r="J14" t="n">
         <v>1</v>
       </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
+      <c r="K14" t="n">
+        <v>25.39999961853027</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.4893680512905121</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2.126389741897583</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>-0.0275401771068573</v>
+      </c>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr">
         <is>
@@ -2159,26 +2272,26 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="2" max="2"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="7" max="7"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="10" max="10"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="16" max="16"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="17" min="17" max="17"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="17" max="17"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="18" max="18"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="19" max="19"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="19" max="19"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="20" max="20"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="21" max="21"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="21" max="21"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="22" max="22"/>
   </cols>
   <sheetData>
@@ -2386,10 +2499,10 @@
         <v>2025020735</v>
       </c>
       <c r="C3" s="7" t="n"/>
-      <c r="D3" s="10" t="n"/>
-      <c r="E3" s="11" t="n"/>
-      <c r="F3" s="11" t="n"/>
-      <c r="G3" s="11" t="n"/>
+      <c r="D3" s="6" t="n"/>
+      <c r="E3" s="5" t="n"/>
+      <c r="F3" s="5" t="n"/>
+      <c r="G3" s="5" t="n"/>
       <c r="H3" s="7" t="inlineStr">
         <is>
           <t>SEA</t>
@@ -2403,21 +2516,21 @@
       <c r="J3" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="10" t="n"/>
-      <c r="L3" s="10" t="n"/>
-      <c r="M3" s="10" t="n"/>
+      <c r="K3" s="6" t="n"/>
+      <c r="L3" s="6" t="n"/>
+      <c r="M3" s="6" t="n"/>
       <c r="N3" s="7" t="n"/>
       <c r="O3" s="7" t="n"/>
-      <c r="P3" s="10" t="n"/>
-      <c r="Q3" s="11" t="n"/>
+      <c r="P3" s="6" t="n"/>
+      <c r="Q3" s="5" t="n"/>
       <c r="R3" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="S3" s="11" t="n"/>
+      <c r="S3" s="5" t="n"/>
       <c r="T3" s="7" t="n"/>
-      <c r="U3" s="11" t="n"/>
+      <c r="U3" s="5" t="n"/>
       <c r="V3" s="7" t="n"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
@@ -2481,7 +2594,7 @@
       <c r="P4" s="6" t="n">
         <v>0.009655356407165527</v>
       </c>
-      <c r="Q4" s="11" t="n"/>
+      <c r="Q4" s="5" t="n"/>
       <c r="R4" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
@@ -2561,7 +2674,7 @@
       <c r="P5" s="6" t="n">
         <v>-0.02398097515106201</v>
       </c>
-      <c r="Q5" s="11" t="n"/>
+      <c r="Q5" s="5" t="n"/>
       <c r="R5" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
@@ -2641,7 +2754,7 @@
       <c r="P6" s="6" t="n">
         <v>-0.02290576696395874</v>
       </c>
-      <c r="Q6" s="11" t="n"/>
+      <c r="Q6" s="5" t="n"/>
       <c r="R6" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
@@ -2670,10 +2783,10 @@
         <v>2025020737</v>
       </c>
       <c r="C7" s="7" t="n"/>
-      <c r="D7" s="10" t="n"/>
-      <c r="E7" s="11" t="n"/>
-      <c r="F7" s="11" t="n"/>
-      <c r="G7" s="11" t="n"/>
+      <c r="D7" s="6" t="n"/>
+      <c r="E7" s="5" t="n"/>
+      <c r="F7" s="5" t="n"/>
+      <c r="G7" s="5" t="n"/>
       <c r="H7" s="7" t="inlineStr">
         <is>
           <t>OTT</t>
@@ -2687,21 +2800,21 @@
       <c r="J7" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="K7" s="10" t="n"/>
-      <c r="L7" s="10" t="n"/>
-      <c r="M7" s="10" t="n"/>
+      <c r="K7" s="6" t="n"/>
+      <c r="L7" s="6" t="n"/>
+      <c r="M7" s="6" t="n"/>
       <c r="N7" s="7" t="n"/>
       <c r="O7" s="7" t="n"/>
-      <c r="P7" s="10" t="n"/>
-      <c r="Q7" s="11" t="n"/>
+      <c r="P7" s="6" t="n"/>
+      <c r="Q7" s="5" t="n"/>
       <c r="R7" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="S7" s="11" t="n"/>
+      <c r="S7" s="5" t="n"/>
       <c r="T7" s="7" t="n"/>
-      <c r="U7" s="11" t="n"/>
+      <c r="U7" s="5" t="n"/>
       <c r="V7" s="7" t="n"/>
     </row>
     <row r="8" ht="18.75" customHeight="1">
@@ -2765,7 +2878,7 @@
       <c r="P8" s="6" t="n">
         <v>-0.02441549301147461</v>
       </c>
-      <c r="Q8" s="11" t="n"/>
+      <c r="Q8" s="5" t="n"/>
       <c r="R8" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
@@ -2845,7 +2958,7 @@
       <c r="P9" s="6" t="n">
         <v>-0.0141146183013916</v>
       </c>
-      <c r="Q9" s="11" t="n"/>
+      <c r="Q9" s="5" t="n"/>
       <c r="R9" s="7" t="inlineStr">
         <is>
           <t>NONE</t>
@@ -2884,26 +2997,26 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="2" max="2"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="7" max="7"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="10" max="10"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="12" max="12"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="13" max="13"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="16" max="16"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="17" max="17"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="17" max="17"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="18" max="18"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="19" max="19"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="19" max="19"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="20" max="20"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="22" min="21" max="21"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="23" min="21" max="21"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="22" max="22"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
feat: update betting tracker
</commit_message>
<xml_diff>
--- a/betting_tracker.xlsx
+++ b/betting_tracker.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="192">
   <si>
     <t>game_date</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>Montembeault</t>
+  </si>
+  <si>
+    <t>Andersen</t>
   </si>
   <si>
     <t>BETTING TRACKER SETTINGS</t>
@@ -652,7 +655,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -682,11 +685,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -712,29 +730,35 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1071,17 +1095,17 @@
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="26" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="A1" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
@@ -1093,10 +1117,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1110,8 +1134,8 @@
       <c r="E4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="22" t="s">
-        <v>168</v>
+      <c r="A5" s="24" t="s">
+        <v>169</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1127,7 +1151,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B7" s="2">
         <v>16</v>
@@ -1138,7 +1162,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B8" s="2">
         <v>9</v>
@@ -1149,7 +1173,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B9" s="2">
         <v>7</v>
@@ -1160,7 +1184,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -1171,10 +1195,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1182,10 +1206,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1193,10 +1217,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1217,8 +1241,8 @@
       <c r="E15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="22" t="s">
-        <v>179</v>
+      <c r="A16" s="24" t="s">
+        <v>180</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1226,20 +1250,20 @@
       <c r="E16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="19" t="s">
-        <v>180</v>
+      <c r="A17" s="21" t="s">
+        <v>181</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>174</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
@@ -1252,11 +1276,11 @@
       <c r="C18" s="2">
         <v>7</v>
       </c>
-      <c r="D18" s="23" t="s">
-        <v>182</v>
+      <c r="D18" s="25" t="s">
+        <v>183</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
@@ -1269,16 +1293,16 @@
       <c r="C19" s="2">
         <v>2</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>184</v>
+      <c r="D19" s="25" t="s">
+        <v>185</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -1286,33 +1310,33 @@
       <c r="C20" s="2">
         <v>0</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>187</v>
+      <c r="D20" s="25" t="s">
+        <v>188</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="B21" s="2">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>187</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -1320,16 +1344,16 @@
       <c r="C22" s="2">
         <v>0</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>187</v>
+      <c r="D22" s="25" t="s">
+        <v>188</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -1337,11 +1361,11 @@
       <c r="C23" s="2">
         <v>0</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>187</v>
+      <c r="D23" s="25" t="s">
+        <v>188</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -4592,8 +4616,8 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="18" t="s">
-        <v>152</v>
+      <c r="A1" s="20" t="s">
+        <v>153</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -4602,16 +4626,16 @@
       <c r="B2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="19" t="s">
-        <v>153</v>
+      <c r="A3" s="21" t="s">
+        <v>154</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -4619,7 +4643,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B5" s="2">
         <v>55</v>
@@ -4627,7 +4651,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B6" s="2">
         <v>65</v>
@@ -4635,7 +4659,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -4647,15 +4671,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B10" s="2">
         <v>-110</v>
@@ -4667,15 +4691,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B13" s="2">
         <v>89</v>
@@ -4691,7 +4715,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -4701,20 +4725,20 @@
     <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -4722,74 +4746,74 @@
     <col min="23" max="23" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4843,9 +4867,9 @@
         <v>29</v>
       </c>
       <c r="Q2" s="13">
-        <v>0.0008561015129089355</v>
-      </c>
-      <c r="R2" s="1"/>
+        <v>0.000856101512909</v>
+      </c>
+      <c r="R2" s="19"/>
       <c r="S2" s="1" t="s">
         <v>30</v>
       </c>
@@ -4906,7 +4930,7 @@
       <c r="Q3" s="13">
         <v>0.019229769706726</v>
       </c>
-      <c r="R3" s="14">
+      <c r="R3" s="12">
         <v>1</v>
       </c>
       <c r="S3" s="1" t="s">
@@ -4969,7 +4993,7 @@
       <c r="Q4" s="13">
         <v>0.0348440408706665</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="12">
         <v>1</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -5032,7 +5056,7 @@
       <c r="Q5" s="13">
         <v>-0.0005941390991210938</v>
       </c>
-      <c r="R5" s="1"/>
+      <c r="R5" s="19"/>
       <c r="S5" s="1" t="s">
         <v>30</v>
       </c>
@@ -5093,7 +5117,7 @@
       <c r="Q6" s="13">
         <v>-0.01791951060295105</v>
       </c>
-      <c r="R6" s="1"/>
+      <c r="R6" s="19"/>
       <c r="S6" s="1" t="s">
         <v>30</v>
       </c>
@@ -5154,7 +5178,7 @@
       <c r="Q7" s="13">
         <v>-0.002641528844833374</v>
       </c>
-      <c r="R7" s="1"/>
+      <c r="R7" s="19"/>
       <c r="S7" s="1" t="s">
         <v>30</v>
       </c>
@@ -5215,7 +5239,7 @@
       <c r="Q8" s="13">
         <v>0.021478354930878</v>
       </c>
-      <c r="R8" s="14">
+      <c r="R8" s="12">
         <v>1</v>
       </c>
       <c r="S8" s="1" t="s">
@@ -5278,7 +5302,7 @@
       <c r="Q9" s="13">
         <v>-0.004612445831298828</v>
       </c>
-      <c r="R9" s="1"/>
+      <c r="R9" s="19"/>
       <c r="S9" s="1" t="s">
         <v>30</v>
       </c>
@@ -5339,7 +5363,7 @@
       <c r="Q10" s="13">
         <v>-0.001081287860870361</v>
       </c>
-      <c r="R10" s="1"/>
+      <c r="R10" s="19"/>
       <c r="S10" s="1" t="s">
         <v>30</v>
       </c>
@@ -5400,7 +5424,7 @@
       <c r="Q11" s="13">
         <v>-0.01918977499008179</v>
       </c>
-      <c r="R11" s="1"/>
+      <c r="R11" s="19"/>
       <c r="S11" s="1" t="s">
         <v>30</v>
       </c>
@@ -5461,7 +5485,7 @@
       <c r="Q12" s="13">
         <v>0.015862464904785</v>
       </c>
-      <c r="R12" s="1"/>
+      <c r="R12" s="19"/>
       <c r="S12" s="1" t="s">
         <v>30</v>
       </c>
@@ -5522,7 +5546,7 @@
       <c r="Q13" s="13">
         <v>-0.01111921668052673</v>
       </c>
-      <c r="R13" s="1"/>
+      <c r="R13" s="19"/>
       <c r="S13" s="1" t="s">
         <v>30</v>
       </c>
@@ -5583,7 +5607,7 @@
       <c r="Q14" s="13">
         <v>0.003808945417404175</v>
       </c>
-      <c r="R14" s="1"/>
+      <c r="R14" s="19"/>
       <c r="S14" s="1" t="s">
         <v>30</v>
       </c>
@@ -5644,7 +5668,7 @@
       <c r="Q15" s="13">
         <v>0.007508993148803711</v>
       </c>
-      <c r="R15" s="1"/>
+      <c r="R15" s="19"/>
       <c r="S15" s="1" t="s">
         <v>30</v>
       </c>
@@ -5705,7 +5729,7 @@
       <c r="Q16" s="13">
         <v>0.0004342198371887207</v>
       </c>
-      <c r="R16" s="1"/>
+      <c r="R16" s="19"/>
       <c r="S16" s="1" t="s">
         <v>30</v>
       </c>
@@ -5713,6 +5737,67 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="12">
+        <v>2025020796</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" s="13">
+        <v>19.5</v>
+      </c>
+      <c r="F17" s="12">
+        <v>-103</v>
+      </c>
+      <c r="G17" s="12">
+        <v>-120</v>
+      </c>
+      <c r="H17" s="12">
+        <v>8475883</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K17" s="12">
+        <v>1</v>
+      </c>
+      <c r="L17" s="13">
+        <v>19.70000076293945</v>
+      </c>
+      <c r="M17" s="13">
+        <v>0.5309252142906189</v>
+      </c>
+      <c r="N17" s="13">
+        <v>6.185042858123779</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="13">
+        <v>0.023536026477814</v>
+      </c>
+      <c r="R17" s="19"/>
+      <c r="S17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5734,20 +5819,20 @@
     <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -5830,7 +5915,7 @@
       <c r="A2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="2">
         <v>2025020789</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -5839,16 +5924,16 @@
       <c r="D2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="3">
         <v>23.5</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="2">
         <v>-107</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="2">
         <v>-115</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="2">
         <v>8475809</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -5857,16 +5942,16 @@
       <c r="J2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="3">
         <v>23.70000076293945</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="3">
         <v>0.5356113314628601</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="3">
         <v>7.122266292572021</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -5875,22 +5960,22 @@
       <c r="P2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="3">
         <v>0.01870310306549072</v>
       </c>
-      <c r="R2" s="12">
+      <c r="R2" s="2">
         <v>1</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="2">
         <v>15</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="V2" s="12">
+      <c r="V2" s="2">
         <v>-1</v>
       </c>
       <c r="W2" s="1"/>
@@ -5899,7 +5984,7 @@
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="2">
         <v>2025020789</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -5908,16 +5993,16 @@
       <c r="D3" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="3">
         <v>27.5</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="2">
         <v>-125</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="2">
         <v>102</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="2">
         <v>8480843</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -5926,16 +6011,16 @@
       <c r="J3" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K3" s="12">
-        <v>0</v>
-      </c>
-      <c r="L3" s="13">
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
         <v>27.29999923706055</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="3">
         <v>0.4652156233787537</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="3">
         <v>6.956875324249268</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -5944,22 +6029,22 @@
       <c r="P3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="3">
         <v>0.03973487019538879</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="2">
         <v>2</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="T3" s="12">
+      <c r="T3" s="2">
         <v>40</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="V3" s="12">
+      <c r="V3" s="2">
         <v>-2</v>
       </c>
       <c r="W3" s="1"/>
@@ -5968,7 +6053,7 @@
       <c r="A4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="2">
         <v>2025020790</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -5977,16 +6062,16 @@
       <c r="D4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="3">
         <v>23.5</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="2">
         <v>-107</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="2">
         <v>-115</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="2">
         <v>8481035</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -5995,16 +6080,16 @@
       <c r="J4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="12">
-        <v>0</v>
-      </c>
-      <c r="L4" s="13">
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
         <v>23.5</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="3">
         <v>0.5046634078025818</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="3">
         <v>0.9326815605163574</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -6013,20 +6098,20 @@
       <c r="P4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="3">
         <v>-0.0122448205947876</v>
       </c>
-      <c r="R4" s="14"/>
+      <c r="R4" s="12"/>
       <c r="S4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T4" s="12">
+      <c r="T4" s="2">
         <v>22</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V4" s="12">
+      <c r="V4" s="2">
         <v>0</v>
       </c>
       <c r="W4" s="1"/>
@@ -6035,7 +6120,7 @@
       <c r="A5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="2">
         <v>2025020793</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -6044,16 +6129,16 @@
       <c r="D5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="3">
         <v>24.5</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="2">
         <v>-102</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="2">
         <v>-122</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="2">
         <v>8475831</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -6062,16 +6147,16 @@
       <c r="J5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="3">
         <v>24.5</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="3">
         <v>0.4978570342063904</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="3">
         <v>0.4285931587219238</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -6080,20 +6165,20 @@
       <c r="P5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="3">
         <v>-0.007093489170074463</v>
       </c>
-      <c r="R5" s="14"/>
+      <c r="R5" s="12"/>
       <c r="S5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T5" s="12">
+      <c r="T5" s="2">
         <v>24</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V5" s="12">
+      <c r="V5" s="2">
         <v>0</v>
       </c>
       <c r="W5" s="1"/>
@@ -6102,7 +6187,7 @@
       <c r="A6" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="2">
         <v>2025020793</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -6111,16 +6196,16 @@
       <c r="D6" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="3">
         <v>24.5</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="2">
         <v>-106</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="2">
         <v>-117</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="2">
         <v>8478009</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -6129,16 +6214,16 @@
       <c r="J6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="12">
-        <v>0</v>
-      </c>
-      <c r="L6" s="13">
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
         <v>24.39999961853027</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="3">
         <v>0.4783008098602295</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="3">
         <v>4.339838027954102</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -6147,20 +6232,20 @@
       <c r="P6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="3">
         <v>-0.0174713134765625</v>
       </c>
-      <c r="R6" s="14"/>
+      <c r="R6" s="12"/>
       <c r="S6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T6" s="12">
+      <c r="T6" s="2">
         <v>21</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V6" s="12">
+      <c r="V6" s="2">
         <v>0</v>
       </c>
       <c r="W6" s="1"/>
@@ -6169,7 +6254,7 @@
       <c r="A7" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="2">
         <v>2025020791</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -6178,16 +6263,16 @@
       <c r="D7" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="3">
         <v>25.5</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="2">
         <v>-115</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="2">
         <v>-107</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="2">
         <v>8481692</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -6196,16 +6281,16 @@
       <c r="J7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="2">
         <v>1</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="3">
         <v>25.5</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="3">
         <v>0.4901162385940552</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="3">
         <v>1.976752281188965</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -6214,20 +6299,20 @@
       <c r="P7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="3">
         <v>-0.007024466991424561</v>
       </c>
-      <c r="R7" s="14"/>
+      <c r="R7" s="12"/>
       <c r="S7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7" s="2">
         <v>21</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V7" s="12">
+      <c r="V7" s="2">
         <v>0</v>
       </c>
       <c r="W7" s="1"/>
@@ -6236,7 +6321,7 @@
       <c r="A8" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="2">
         <v>2025020791</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -6245,16 +6330,16 @@
       <c r="D8" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="3">
         <v>24.5</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="2">
         <v>-104</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="2">
         <v>-118</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="2">
         <v>8479973</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -6263,16 +6348,16 @@
       <c r="J8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="13">
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
         <v>24.29999923706055</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="3">
         <v>0.4680142998695374</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="3">
         <v>6.397140026092529</v>
       </c>
       <c r="O8" s="1" t="s">
@@ -6281,20 +6366,20 @@
       <c r="P8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="3">
         <v>-0.00929868221282959</v>
       </c>
-      <c r="R8" s="14"/>
+      <c r="R8" s="12"/>
       <c r="S8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T8" s="12">
+      <c r="T8" s="2">
         <v>18</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V8" s="12">
+      <c r="V8" s="2">
         <v>0</v>
       </c>
       <c r="W8" s="1"/>
@@ -6303,7 +6388,7 @@
       <c r="A9" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="2">
         <v>2025020792</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -6312,16 +6397,16 @@
       <c r="D9" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="3">
         <v>24.5</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="2">
         <v>-113</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="2">
         <v>-109</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="2">
         <v>8480947</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -6330,16 +6415,16 @@
       <c r="J9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="2">
         <v>1</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="3">
         <v>24.39999961853027</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="3">
         <v>0.4808475077152252</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="3">
         <v>3.830498456954956</v>
       </c>
       <c r="O9" s="1" t="s">
@@ -6348,20 +6433,20 @@
       <c r="P9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="3">
         <v>-0.002378582954406738</v>
       </c>
-      <c r="R9" s="14"/>
+      <c r="R9" s="12"/>
       <c r="S9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T9" s="12">
+      <c r="T9" s="2">
         <v>29</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V9" s="12">
+      <c r="V9" s="2">
         <v>0</v>
       </c>
       <c r="W9" s="1"/>
@@ -6370,7 +6455,7 @@
       <c r="A10" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="2">
         <v>2025020792</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -6379,16 +6464,16 @@
       <c r="D10" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="3">
         <v>24.5</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="2">
         <v>-106</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="2">
         <v>-115</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="2">
         <v>8480313</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -6397,16 +6482,16 @@
       <c r="J10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="12">
-        <v>0</v>
-      </c>
-      <c r="L10" s="13">
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
         <v>24.39999961853027</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="3">
         <v>0.4860748648643494</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="3">
         <v>2.785027027130127</v>
       </c>
       <c r="O10" s="1" t="s">
@@ -6415,20 +6500,20 @@
       <c r="P10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="3">
         <v>-0.02095860242843628</v>
       </c>
-      <c r="R10" s="14"/>
+      <c r="R10" s="12"/>
       <c r="S10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T10" s="12">
+      <c r="T10" s="2">
         <v>21</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V10" s="12">
+      <c r="V10" s="2">
         <v>0</v>
       </c>
       <c r="W10" s="1"/>
@@ -6437,7 +6522,7 @@
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="2">
         <v>2025020789</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -6446,10 +6531,10 @@
       <c r="D11" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="12">
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="2">
         <v>8475809</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -6458,26 +6543,26 @@
       <c r="J11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="2">
         <v>1</v>
       </c>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="14"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="12"/>
       <c r="S11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T11" s="12">
+      <c r="T11" s="2">
         <v>15</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V11" s="12">
+      <c r="V11" s="2">
         <v>0</v>
       </c>
       <c r="W11" s="1"/>
@@ -6486,7 +6571,7 @@
       <c r="A12" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="2">
         <v>2025020789</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -6495,10 +6580,10 @@
       <c r="D12" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="12">
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="2">
         <v>8480843</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -6507,26 +6592,26 @@
       <c r="J12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K12" s="12">
-        <v>0</v>
-      </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="14"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="12"/>
       <c r="S12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T12" s="12">
+      <c r="T12" s="2">
         <v>40</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V12" s="12">
+      <c r="V12" s="2">
         <v>0</v>
       </c>
       <c r="W12" s="1"/>
@@ -6535,7 +6620,7 @@
       <c r="A13" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="2">
         <v>2025020790</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -6544,10 +6629,10 @@
       <c r="D13" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="12">
+      <c r="E13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="2">
         <v>8481035</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -6556,26 +6641,26 @@
       <c r="J13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="12">
-        <v>0</v>
-      </c>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="14"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="12"/>
       <c r="S13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T13" s="12">
+      <c r="T13" s="2">
         <v>22</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V13" s="12">
+      <c r="V13" s="2">
         <v>0</v>
       </c>
       <c r="W13" s="1"/>
@@ -6584,7 +6669,7 @@
       <c r="A14" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="2">
         <v>2025020793</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -6593,10 +6678,10 @@
       <c r="D14" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="12">
+      <c r="E14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="2">
         <v>8475831</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -6605,26 +6690,26 @@
       <c r="J14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="2">
         <v>1</v>
       </c>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="14"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="12"/>
       <c r="S14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T14" s="12">
+      <c r="T14" s="2">
         <v>24</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V14" s="12">
+      <c r="V14" s="2">
         <v>0</v>
       </c>
       <c r="W14" s="1"/>
@@ -6633,7 +6718,7 @@
       <c r="A15" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="2">
         <v>2025020793</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -6642,10 +6727,10 @@
       <c r="D15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="12">
+      <c r="E15" s="13"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="2">
         <v>8478009</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -6654,26 +6739,26 @@
       <c r="J15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="12">
-        <v>0</v>
-      </c>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="14"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="12"/>
       <c r="S15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T15" s="12">
+      <c r="T15" s="2">
         <v>21</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V15" s="12">
+      <c r="V15" s="2">
         <v>0</v>
       </c>
       <c r="W15" s="1"/>
@@ -6682,7 +6767,7 @@
       <c r="A16" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="2">
         <v>2025020791</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -6691,10 +6776,10 @@
       <c r="D16" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="12">
+      <c r="E16" s="13"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="2">
         <v>8481692</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -6703,26 +6788,26 @@
       <c r="J16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="2">
         <v>1</v>
       </c>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="14"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="12"/>
       <c r="S16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T16" s="12">
+      <c r="T16" s="2">
         <v>21</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V16" s="12">
+      <c r="V16" s="2">
         <v>0</v>
       </c>
       <c r="W16" s="1"/>
@@ -6731,7 +6816,7 @@
       <c r="A17" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="2">
         <v>2025020791</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -6740,10 +6825,10 @@
       <c r="D17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="12">
+      <c r="E17" s="13"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="2">
         <v>8479973</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -6752,26 +6837,26 @@
       <c r="J17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="14"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="12"/>
       <c r="S17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T17" s="12">
+      <c r="T17" s="2">
         <v>18</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V17" s="12">
+      <c r="V17" s="2">
         <v>0</v>
       </c>
       <c r="W17" s="1"/>
@@ -6780,7 +6865,7 @@
       <c r="A18" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="2">
         <v>2025020792</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -6789,10 +6874,10 @@
       <c r="D18" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="12">
+      <c r="E18" s="13"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="2">
         <v>8480947</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -6801,26 +6886,26 @@
       <c r="J18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="2">
         <v>1</v>
       </c>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="14"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="12"/>
       <c r="S18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T18" s="12">
+      <c r="T18" s="2">
         <v>29</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V18" s="12">
+      <c r="V18" s="2">
         <v>0</v>
       </c>
       <c r="W18" s="1"/>
@@ -6829,7 +6914,7 @@
       <c r="A19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="2">
         <v>2025020792</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -6838,10 +6923,10 @@
       <c r="D19" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="12">
+      <c r="E19" s="13"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="2">
         <v>8480313</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -6850,26 +6935,26 @@
       <c r="J19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="12">
-        <v>0</v>
-      </c>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="14"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="12"/>
       <c r="S19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T19" s="12">
+      <c r="T19" s="2">
         <v>21</v>
       </c>
       <c r="U19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V19" s="12">
+      <c r="V19" s="2">
         <v>0</v>
       </c>
       <c r="W19" s="1"/>

</xml_diff>

<commit_message>
feat: added prizepicks lines
</commit_message>
<xml_diff>
--- a/betting_tracker.xlsx
+++ b/betting_tracker.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="192">
   <si>
     <t>game_date</t>
   </si>
@@ -704,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -739,26 +739,23 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1095,17 +1092,17 @@
     <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="26" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="25" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
@@ -1134,7 +1131,7 @@
       <c r="E4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>169</v>
       </c>
       <c r="B5" s="2"/>
@@ -1241,7 +1238,7 @@
       <c r="E15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>180</v>
       </c>
       <c r="B16" s="2"/>
@@ -1250,7 +1247,7 @@
       <c r="E16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="20" t="s">
         <v>181</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1259,7 +1256,7 @@
       <c r="C17" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="20" t="s">
         <v>174</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1276,7 +1273,7 @@
       <c r="C18" s="2">
         <v>7</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="24" t="s">
         <v>183</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1293,7 +1290,7 @@
       <c r="C19" s="2">
         <v>2</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="24" t="s">
         <v>185</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -1310,7 +1307,7 @@
       <c r="C20" s="2">
         <v>0</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="24" t="s">
         <v>188</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1327,7 +1324,7 @@
       <c r="C21" s="2">
         <v>0</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="24" t="s">
         <v>188</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -1344,7 +1341,7 @@
       <c r="C22" s="2">
         <v>0</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="24" t="s">
         <v>188</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -1361,7 +1358,7 @@
       <c r="C23" s="2">
         <v>0</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="24" t="s">
         <v>188</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -4616,7 +4613,7 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>153</v>
       </c>
       <c r="B1" s="2"/>
@@ -4626,7 +4623,7 @@
       <c r="B2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>154</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -4715,7 +4712,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -4725,20 +4722,20 @@
     <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="7" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -4747,73 +4744,73 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="U1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="V1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="W1" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4821,7 +4818,7 @@
       <c r="A2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="15">
         <v>2025020794</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -4830,16 +4827,16 @@
       <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="16">
         <v>21.5</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="15">
         <v>-114</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="15">
         <v>-108</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="15">
         <v>8481033</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -4848,16 +4845,16 @@
       <c r="J2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="12">
-        <v>0</v>
-      </c>
-      <c r="L2" s="13">
+      <c r="K2" s="15">
+        <v>0</v>
+      </c>
+      <c r="L2" s="16">
         <v>21.70000076293945</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="16">
         <v>0.5335663557052612</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="16">
         <v>6.713271141052246</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -4866,10 +4863,10 @@
       <c r="P2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="16">
         <v>0.000856101512909</v>
       </c>
-      <c r="R2" s="19"/>
+      <c r="R2" s="17"/>
       <c r="S2" s="1" t="s">
         <v>30</v>
       </c>
@@ -4882,7 +4879,7 @@
       <c r="A3" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="15">
         <v>2025020794</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -4891,16 +4888,16 @@
       <c r="D3" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="16">
         <v>24.5</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="15">
         <v>-114</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="15">
         <v>-108</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="15">
         <v>8476914</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -4909,16 +4906,16 @@
       <c r="J3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="15">
         <v>1</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="16">
         <v>24.29999923706055</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="16">
         <v>0.4615394473075867</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="16">
         <v>7.692110538482666</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -4927,10 +4924,10 @@
       <c r="P3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="16">
         <v>0.019229769706726</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="15">
         <v>1</v>
       </c>
       <c r="S3" s="1" t="s">
@@ -4945,7 +4942,7 @@
       <c r="A4" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="15">
         <v>2025020796</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -4954,16 +4951,16 @@
       <c r="D4" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="16">
         <v>27.5</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="15">
         <v>-122</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="15">
         <v>100</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="15">
         <v>8481519</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -4972,28 +4969,28 @@
       <c r="J4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="12">
-        <v>0</v>
-      </c>
-      <c r="L4" s="13">
-        <v>27.29999923706055</v>
-      </c>
-      <c r="M4" s="13">
+      <c r="K4" s="15">
+        <v>0</v>
+      </c>
+      <c r="L4" s="16">
+        <v>28.29999923706055</v>
+      </c>
+      <c r="M4" s="16">
         <v>0.4651559293270111</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="16">
         <v>6.968813896179199</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q4" s="13">
-        <v>0.0348440408706665</v>
-      </c>
-      <c r="R4" s="12">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="16">
+        <v>0.0065421462059021</v>
+      </c>
+      <c r="R4" s="15">
         <v>1</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -5008,7 +5005,7 @@
       <c r="A5" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="15">
         <v>2025020797</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -5017,16 +5014,16 @@
       <c r="D5" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="16">
         <v>23.5</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="15">
         <v>-114</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="15">
         <v>-108</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="15">
         <v>8482982</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -5035,16 +5032,16 @@
       <c r="J5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="15">
         <v>1</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="16">
         <v>23.70000076293945</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="16">
         <v>0.5321161150932312</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="16">
         <v>6.42322301864624</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -5053,10 +5050,10 @@
       <c r="P5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="16">
         <v>-0.0005941390991210938</v>
       </c>
-      <c r="R5" s="19"/>
+      <c r="R5" s="17"/>
       <c r="S5" s="1" t="s">
         <v>30</v>
       </c>
@@ -5069,7 +5066,7 @@
       <c r="A6" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="15">
         <v>2025020797</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -5078,16 +5075,16 @@
       <c r="D6" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="16">
         <v>25.5</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="15">
         <v>-105</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="15">
         <v>-118</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="15">
         <v>8479193</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -5096,16 +5093,16 @@
       <c r="J6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="12">
-        <v>0</v>
-      </c>
-      <c r="L6" s="13">
+      <c r="K6" s="15">
+        <v>0</v>
+      </c>
+      <c r="L6" s="16">
         <v>25.5</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="16">
         <v>0.4942755997180939</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="16">
         <v>1.144880056381226</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -5114,10 +5111,10 @@
       <c r="P6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="16">
         <v>-0.01791951060295105</v>
       </c>
-      <c r="R6" s="19"/>
+      <c r="R6" s="17"/>
       <c r="S6" s="1" t="s">
         <v>30</v>
       </c>
@@ -5130,7 +5127,7 @@
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="15">
         <v>2025020799</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -5139,16 +5136,16 @@
       <c r="D7" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="16">
         <v>25.5</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="15">
         <v>101</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="15">
         <v>-124</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="15">
         <v>8476945</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -5157,16 +5154,16 @@
       <c r="J7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="15">
         <v>1</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="16">
         <v>25.5</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="16">
         <v>0.4948709011077881</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="16">
         <v>1.025819778442383</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -5175,10 +5172,10 @@
       <c r="P7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="13">
-        <v>-0.002641528844833374</v>
-      </c>
-      <c r="R7" s="19"/>
+      <c r="Q7" s="16">
+        <v>0.002260059118270874</v>
+      </c>
+      <c r="R7" s="17"/>
       <c r="S7" s="1" t="s">
         <v>30</v>
       </c>
@@ -5191,7 +5188,7 @@
       <c r="A8" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="15">
         <v>2025020799</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -5200,16 +5197,16 @@
       <c r="D8" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="16">
         <v>22.5</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="15">
         <v>-103</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="15">
         <v>-120</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="15">
         <v>8480193</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -5218,16 +5215,16 @@
       <c r="J8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="13">
+      <c r="K8" s="15">
+        <v>0</v>
+      </c>
+      <c r="L8" s="16">
         <v>22.60000038146973</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="16">
         <v>0.5288675427436829</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="16">
         <v>5.773508548736572</v>
       </c>
       <c r="O8" s="1" t="s">
@@ -5236,10 +5233,10 @@
       <c r="P8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="16">
         <v>0.021478354930878</v>
       </c>
-      <c r="R8" s="12">
+      <c r="R8" s="15">
         <v>1</v>
       </c>
       <c r="S8" s="1" t="s">
@@ -5254,7 +5251,7 @@
       <c r="A9" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="15">
         <v>2025020798</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -5263,16 +5260,16 @@
       <c r="D9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="16">
         <v>24.5</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="15">
         <v>-122</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="15">
         <v>100</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="15">
         <v>8477424</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -5281,16 +5278,16 @@
       <c r="J9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="15">
         <v>1</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="16">
         <v>24.5</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="16">
         <v>0.5046124458312988</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="16">
         <v>0.9224891662597656</v>
       </c>
       <c r="O9" s="1" t="s">
@@ -5299,10 +5296,10 @@
       <c r="P9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="16">
         <v>-0.004612445831298828</v>
       </c>
-      <c r="R9" s="19"/>
+      <c r="R9" s="17"/>
       <c r="S9" s="1" t="s">
         <v>30</v>
       </c>
@@ -5315,7 +5312,7 @@
       <c r="A10" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="15">
         <v>2025020798</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -5324,16 +5321,16 @@
       <c r="D10" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="16">
         <v>23.5</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="15">
         <v>-108</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="15">
         <v>-114</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="15">
         <v>8473503</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -5342,16 +5339,16 @@
       <c r="J10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="12">
-        <v>0</v>
-      </c>
-      <c r="L10" s="13">
+      <c r="K10" s="15">
+        <v>0</v>
+      </c>
+      <c r="L10" s="16">
         <v>23.60000038146973</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="16">
         <v>0.5181494951248169</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="16">
         <v>3.629899024963379</v>
       </c>
       <c r="O10" s="1" t="s">
@@ -5360,10 +5357,10 @@
       <c r="P10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="16">
         <v>-0.001081287860870361</v>
       </c>
-      <c r="R10" s="19"/>
+      <c r="R10" s="17"/>
       <c r="S10" s="1" t="s">
         <v>30</v>
       </c>
@@ -5376,7 +5373,7 @@
       <c r="A11" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="15">
         <v>2025020800</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -5385,16 +5382,16 @@
       <c r="D11" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="16">
         <v>24.5</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="15">
         <v>-110</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="15">
         <v>-112</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="15">
         <v>8481668</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -5403,16 +5400,16 @@
       <c r="J11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="12">
-        <v>0</v>
-      </c>
-      <c r="L11" s="13">
+      <c r="K11" s="15">
+        <v>0</v>
+      </c>
+      <c r="L11" s="16">
         <v>24.5</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="16">
         <v>0.4908878803253174</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="16">
         <v>1.822423934936523</v>
       </c>
       <c r="O11" s="1" t="s">
@@ -5421,10 +5418,10 @@
       <c r="P11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q11" s="13">
+      <c r="Q11" s="16">
         <v>-0.01918977499008179</v>
       </c>
-      <c r="R11" s="19"/>
+      <c r="R11" s="17"/>
       <c r="S11" s="1" t="s">
         <v>30</v>
       </c>
@@ -5437,7 +5434,7 @@
       <c r="A12" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="15">
         <v>2025020800</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -5446,16 +5443,16 @@
       <c r="D12" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="16">
         <v>23.5</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="15">
         <v>-107</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="15">
         <v>-115</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="15">
         <v>8477465</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -5464,16 +5461,16 @@
       <c r="J12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="15">
         <v>1</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="16">
         <v>23.70000076293945</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="16">
         <v>0.5327706933021545</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="16">
         <v>6.554138660430908</v>
       </c>
       <c r="O12" s="1" t="s">
@@ -5482,10 +5479,10 @@
       <c r="P12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q12" s="13">
+      <c r="Q12" s="16">
         <v>0.015862464904785</v>
       </c>
-      <c r="R12" s="19"/>
+      <c r="R12" s="17"/>
       <c r="S12" s="1" t="s">
         <v>30</v>
       </c>
@@ -5498,7 +5495,7 @@
       <c r="A13" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="15">
         <v>2025020801</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -5507,16 +5504,16 @@
       <c r="D13" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="16">
         <v>25.5</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="15">
         <v>101</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="15">
         <v>-124</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="15">
         <v>8475660</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -5525,16 +5522,16 @@
       <c r="J13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K13" s="12">
-        <v>0</v>
-      </c>
-      <c r="L13" s="13">
+      <c r="K13" s="15">
+        <v>0</v>
+      </c>
+      <c r="L13" s="16">
         <v>25.39999961853027</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="16">
         <v>0.4863932132720947</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="16">
         <v>2.721357345581055</v>
       </c>
       <c r="O13" s="1" t="s">
@@ -5543,10 +5540,10 @@
       <c r="P13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="Q13" s="16">
         <v>-0.01111921668052673</v>
       </c>
-      <c r="R13" s="19"/>
+      <c r="R13" s="17"/>
       <c r="S13" s="1" t="s">
         <v>30</v>
       </c>
@@ -5559,7 +5556,7 @@
       <c r="A14" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="15">
         <v>2025020801</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -5568,16 +5565,16 @@
       <c r="D14" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="16">
         <v>24.5</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="15">
         <v>101</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="15">
         <v>-124</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="15">
         <v>8479406</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -5586,16 +5583,16 @@
       <c r="J14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="15">
         <v>1</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="16">
         <v>24.5</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="16">
         <v>0.5013213753700256</v>
       </c>
-      <c r="N14" s="13">
+      <c r="N14" s="16">
         <v>0.264275074005127</v>
       </c>
       <c r="O14" s="1" t="s">
@@ -5604,10 +5601,10 @@
       <c r="P14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="Q14" s="16">
         <v>0.003808945417404175</v>
       </c>
-      <c r="R14" s="19"/>
+      <c r="R14" s="17"/>
       <c r="S14" s="1" t="s">
         <v>30</v>
       </c>
@@ -5620,7 +5617,7 @@
       <c r="A15" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="15">
         <v>2025020795</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -5629,16 +5626,16 @@
       <c r="D15" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="16">
         <v>22.5</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="15">
         <v>-112</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="15">
         <v>-110</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="15">
         <v>8478470</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -5647,16 +5644,16 @@
       <c r="J15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="15">
         <v>1</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="16">
         <v>22.70000076293945</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="16">
         <v>0.5358108878135681</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="16">
         <v>7.162177562713623</v>
       </c>
       <c r="O15" s="1" t="s">
@@ -5665,10 +5662,10 @@
       <c r="P15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q15" s="13">
+      <c r="Q15" s="16">
         <v>0.007508993148803711</v>
       </c>
-      <c r="R15" s="19"/>
+      <c r="R15" s="17"/>
       <c r="S15" s="1" t="s">
         <v>30</v>
       </c>
@@ -5681,7 +5678,7 @@
       <c r="A16" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="15">
         <v>2025020795</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -5690,16 +5687,16 @@
       <c r="D16" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="16">
         <v>24.5</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="15">
         <v>-112</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="15">
         <v>-110</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="15">
         <v>8480045</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -5708,16 +5705,16 @@
       <c r="J16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="12">
-        <v>0</v>
-      </c>
-      <c r="L16" s="13">
+      <c r="K16" s="15">
+        <v>0</v>
+      </c>
+      <c r="L16" s="16">
         <v>24.39999961853027</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="16">
         <v>0.4757562279701233</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="16">
         <v>4.848754405975342</v>
       </c>
       <c r="O16" s="1" t="s">
@@ -5726,10 +5723,10 @@
       <c r="P16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q16" s="13">
+      <c r="Q16" s="16">
         <v>0.0004342198371887207</v>
       </c>
-      <c r="R16" s="19"/>
+      <c r="R16" s="17"/>
       <c r="S16" s="1" t="s">
         <v>30</v>
       </c>
@@ -5742,7 +5739,7 @@
       <c r="A17" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="15">
         <v>2025020796</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -5751,16 +5748,16 @@
       <c r="D17" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="16">
         <v>19.5</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="15">
         <v>-103</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="15">
         <v>-120</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="15">
         <v>8475883</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -5769,16 +5766,16 @@
       <c r="J17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="15">
         <v>1</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="16">
         <v>19.70000076293945</v>
       </c>
-      <c r="M17" s="13">
+      <c r="M17" s="16">
         <v>0.5309252142906189</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="16">
         <v>6.185042858123779</v>
       </c>
       <c r="O17" s="1" t="s">
@@ -5787,10 +5784,10 @@
       <c r="P17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q17" s="13">
-        <v>0.023536026477814</v>
-      </c>
-      <c r="R17" s="19"/>
+      <c r="Q17" s="16">
+        <v>0.03587570786476135</v>
+      </c>
+      <c r="R17" s="17"/>
       <c r="S17" s="1" t="s">
         <v>30</v>
       </c>
@@ -5798,6 +5795,801 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="15">
+        <v>2025020796</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="16">
+        <v>28.5</v>
+      </c>
+      <c r="F18" s="15">
+        <v>-112</v>
+      </c>
+      <c r="G18" s="15">
+        <v>-112</v>
+      </c>
+      <c r="H18" s="15">
+        <v>8481519</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" s="15">
+        <v>0</v>
+      </c>
+      <c r="L18" s="16">
+        <v>28.29999923706055</v>
+      </c>
+      <c r="M18" s="16">
+        <v>0.4651559293270111</v>
+      </c>
+      <c r="N18" s="16">
+        <v>6.968813896179199</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q18" s="16">
+        <v>0.0065421462059021</v>
+      </c>
+      <c r="R18" s="17"/>
+      <c r="S18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="15">
+        <v>2025020796</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="16">
+        <v>19.5</v>
+      </c>
+      <c r="F19" s="15">
+        <v>102</v>
+      </c>
+      <c r="G19" s="15">
+        <v>-125</v>
+      </c>
+      <c r="H19" s="15">
+        <v>8475883</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" s="15">
+        <v>1</v>
+      </c>
+      <c r="L19" s="16">
+        <v>19.70000076293945</v>
+      </c>
+      <c r="M19" s="16">
+        <v>0.5309252142906189</v>
+      </c>
+      <c r="N19" s="16">
+        <v>6.185042858123779</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q19" s="16">
+        <v>0.03587570786476135</v>
+      </c>
+      <c r="R19" s="15">
+        <v>1</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="15">
+        <v>2025020799</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="16">
+        <v>25.5</v>
+      </c>
+      <c r="F20" s="15">
+        <v>103</v>
+      </c>
+      <c r="G20" s="15">
+        <v>-124</v>
+      </c>
+      <c r="H20" s="15">
+        <v>8476945</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K20" s="15">
+        <v>1</v>
+      </c>
+      <c r="L20" s="16">
+        <v>25.5</v>
+      </c>
+      <c r="M20" s="16">
+        <v>0.4948709011077881</v>
+      </c>
+      <c r="N20" s="16">
+        <v>1.025819778442383</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>0.002260059118270874</v>
+      </c>
+      <c r="R20" s="17"/>
+      <c r="S20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="15">
+        <v>2025020799</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="16">
+        <v>25.5</v>
+      </c>
+      <c r="F21" s="15">
+        <v>103</v>
+      </c>
+      <c r="G21" s="15">
+        <v>-124</v>
+      </c>
+      <c r="H21" s="15">
+        <v>8476945</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K21" s="15">
+        <v>1</v>
+      </c>
+      <c r="L21" s="16">
+        <v>25.5</v>
+      </c>
+      <c r="M21" s="16">
+        <v>0.4948709011077881</v>
+      </c>
+      <c r="N21" s="16">
+        <v>1.025819778442383</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q21" s="16">
+        <v>0.002260059118270874</v>
+      </c>
+      <c r="R21" s="17"/>
+      <c r="S21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="15">
+        <v>2025020799</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" s="16">
+        <v>25.5</v>
+      </c>
+      <c r="F22" s="15">
+        <v>103</v>
+      </c>
+      <c r="G22" s="15">
+        <v>-124</v>
+      </c>
+      <c r="H22" s="15">
+        <v>8476945</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K22" s="15">
+        <v>1</v>
+      </c>
+      <c r="L22" s="16">
+        <v>25.5</v>
+      </c>
+      <c r="M22" s="16">
+        <v>0.4948709011077881</v>
+      </c>
+      <c r="N22" s="16">
+        <v>1.025819778442383</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q22" s="16">
+        <v>0.002260059118270874</v>
+      </c>
+      <c r="R22" s="17"/>
+      <c r="S22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" s="15">
+        <v>2025020798</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="15">
+        <v>25</v>
+      </c>
+      <c r="F23" s="15">
+        <v>-120</v>
+      </c>
+      <c r="G23" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H23" s="15">
+        <v>8477424</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="15">
+        <v>1</v>
+      </c>
+      <c r="L23" s="15">
+        <v>25</v>
+      </c>
+      <c r="M23" s="16">
+        <v>0.5045216679573059</v>
+      </c>
+      <c r="N23" s="16">
+        <v>0.9043335914611816</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q23" s="16">
+        <v>-0.04093289375305176</v>
+      </c>
+      <c r="R23" s="17"/>
+      <c r="S23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="15">
+        <v>2025020798</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="16">
+        <v>23.5</v>
+      </c>
+      <c r="F24" s="15">
+        <v>-120</v>
+      </c>
+      <c r="G24" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H24" s="15">
+        <v>8473503</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K24" s="15">
+        <v>0</v>
+      </c>
+      <c r="L24" s="16">
+        <v>23.60000038146973</v>
+      </c>
+      <c r="M24" s="16">
+        <v>0.5181494951248169</v>
+      </c>
+      <c r="N24" s="16">
+        <v>3.629899024963379</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q24" s="16">
+        <v>-0.02730506658554077</v>
+      </c>
+      <c r="R24" s="17"/>
+      <c r="S24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="15">
+        <v>2025020799</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="15">
+        <v>25</v>
+      </c>
+      <c r="F25" s="15">
+        <v>-120</v>
+      </c>
+      <c r="G25" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H25" s="15">
+        <v>8476945</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K25" s="15">
+        <v>1</v>
+      </c>
+      <c r="L25" s="15">
+        <v>25</v>
+      </c>
+      <c r="M25" s="16">
+        <v>0.4971076548099518</v>
+      </c>
+      <c r="N25" s="16">
+        <v>0.5784690380096436</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q25" s="16">
+        <v>-0.04256218671798706</v>
+      </c>
+      <c r="R25" s="17"/>
+      <c r="S25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="15">
+        <v>2025020799</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="16">
+        <v>22.5</v>
+      </c>
+      <c r="F26" s="15">
+        <v>-120</v>
+      </c>
+      <c r="G26" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H26" s="15">
+        <v>8480193</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K26" s="15">
+        <v>0</v>
+      </c>
+      <c r="L26" s="16">
+        <v>22.60000038146973</v>
+      </c>
+      <c r="M26" s="16">
+        <v>0.5288675427436829</v>
+      </c>
+      <c r="N26" s="16">
+        <v>5.773508548736572</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q26" s="16">
+        <v>-0.0165870189666748</v>
+      </c>
+      <c r="R26" s="17"/>
+      <c r="S26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="15">
+        <v>2025020800</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="16">
+        <v>24.5</v>
+      </c>
+      <c r="F27" s="15">
+        <v>-120</v>
+      </c>
+      <c r="G27" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H27" s="15">
+        <v>8481668</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K27" s="15">
+        <v>0</v>
+      </c>
+      <c r="L27" s="16">
+        <v>24.5</v>
+      </c>
+      <c r="M27" s="16">
+        <v>0.4908878803253174</v>
+      </c>
+      <c r="N27" s="16">
+        <v>1.822423934936523</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q27" s="16">
+        <v>-0.03634244203567505</v>
+      </c>
+      <c r="R27" s="17"/>
+      <c r="S27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="15">
+        <v>2025020800</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" s="16">
+        <v>23.5</v>
+      </c>
+      <c r="F28" s="15">
+        <v>-120</v>
+      </c>
+      <c r="G28" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H28" s="15">
+        <v>8477465</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="15">
+        <v>1</v>
+      </c>
+      <c r="L28" s="16">
+        <v>23.70000076293945</v>
+      </c>
+      <c r="M28" s="16">
+        <v>0.5327706933021545</v>
+      </c>
+      <c r="N28" s="16">
+        <v>6.554138660430908</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q28" s="16">
+        <v>-0.01268386840820312</v>
+      </c>
+      <c r="R28" s="17"/>
+      <c r="S28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="15">
+        <v>2025020801</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="15">
+        <v>25</v>
+      </c>
+      <c r="F29" s="15">
+        <v>-120</v>
+      </c>
+      <c r="G29" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H29" s="15">
+        <v>8475660</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K29" s="15">
+        <v>0</v>
+      </c>
+      <c r="L29" s="16">
+        <v>24.89999961853027</v>
+      </c>
+      <c r="M29" s="16">
+        <v>0.4886287450790405</v>
+      </c>
+      <c r="N29" s="16">
+        <v>2.274250984191895</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q29" s="16">
+        <v>-0.03408330678939819</v>
+      </c>
+      <c r="R29" s="17"/>
+      <c r="S29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="15">
+        <v>2025020801</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="15">
+        <v>24</v>
+      </c>
+      <c r="F30" s="15">
+        <v>-120</v>
+      </c>
+      <c r="G30" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H30" s="15">
+        <v>8479406</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K30" s="15">
+        <v>1</v>
+      </c>
+      <c r="L30" s="15">
+        <v>24</v>
+      </c>
+      <c r="M30" s="16">
+        <v>0.5077030658721924</v>
+      </c>
+      <c r="N30" s="16">
+        <v>1.540613174438477</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q30" s="16">
+        <v>-0.03775149583816528</v>
+      </c>
+      <c r="R30" s="17"/>
+      <c r="S30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5819,20 +6611,20 @@
     <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -6101,7 +6893,7 @@
       <c r="Q4" s="3">
         <v>-0.0122448205947876</v>
       </c>
-      <c r="R4" s="12"/>
+      <c r="R4" s="2"/>
       <c r="S4" s="1" t="s">
         <v>30</v>
       </c>
@@ -6168,7 +6960,7 @@
       <c r="Q5" s="3">
         <v>-0.007093489170074463</v>
       </c>
-      <c r="R5" s="12"/>
+      <c r="R5" s="2"/>
       <c r="S5" s="1" t="s">
         <v>30</v>
       </c>
@@ -6235,7 +7027,7 @@
       <c r="Q6" s="3">
         <v>-0.0174713134765625</v>
       </c>
-      <c r="R6" s="12"/>
+      <c r="R6" s="2"/>
       <c r="S6" s="1" t="s">
         <v>30</v>
       </c>
@@ -6302,7 +7094,7 @@
       <c r="Q7" s="3">
         <v>-0.007024466991424561</v>
       </c>
-      <c r="R7" s="12"/>
+      <c r="R7" s="2"/>
       <c r="S7" s="1" t="s">
         <v>30</v>
       </c>
@@ -6369,7 +7161,7 @@
       <c r="Q8" s="3">
         <v>-0.00929868221282959</v>
       </c>
-      <c r="R8" s="12"/>
+      <c r="R8" s="2"/>
       <c r="S8" s="1" t="s">
         <v>30</v>
       </c>
@@ -6436,7 +7228,7 @@
       <c r="Q9" s="3">
         <v>-0.002378582954406738</v>
       </c>
-      <c r="R9" s="12"/>
+      <c r="R9" s="2"/>
       <c r="S9" s="1" t="s">
         <v>30</v>
       </c>
@@ -6503,7 +7295,7 @@
       <c r="Q10" s="3">
         <v>-0.02095860242843628</v>
       </c>
-      <c r="R10" s="12"/>
+      <c r="R10" s="2"/>
       <c r="S10" s="1" t="s">
         <v>30</v>
       </c>
@@ -6531,9 +7323,9 @@
       <c r="D11" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2">
         <v>8475809</v>
       </c>
@@ -6546,13 +7338,13 @@
       <c r="K11" s="2">
         <v>1</v>
       </c>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="12"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="2"/>
       <c r="S11" s="1" t="s">
         <v>30</v>
       </c>
@@ -6580,9 +7372,9 @@
       <c r="D12" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="2">
         <v>8480843</v>
       </c>
@@ -6595,13 +7387,13 @@
       <c r="K12" s="2">
         <v>0</v>
       </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="12"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="2"/>
       <c r="S12" s="1" t="s">
         <v>30</v>
       </c>
@@ -6629,9 +7421,9 @@
       <c r="D13" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
       <c r="H13" s="2">
         <v>8481035</v>
       </c>
@@ -6644,13 +7436,13 @@
       <c r="K13" s="2">
         <v>0</v>
       </c>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="12"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="2"/>
       <c r="S13" s="1" t="s">
         <v>30</v>
       </c>
@@ -6678,9 +7470,9 @@
       <c r="D14" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2">
         <v>8475831</v>
       </c>
@@ -6693,13 +7485,13 @@
       <c r="K14" s="2">
         <v>1</v>
       </c>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="12"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="2"/>
       <c r="S14" s="1" t="s">
         <v>30</v>
       </c>
@@ -6727,9 +7519,9 @@
       <c r="D15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="2">
         <v>8478009</v>
       </c>
@@ -6742,13 +7534,13 @@
       <c r="K15" s="2">
         <v>0</v>
       </c>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="12"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="2"/>
       <c r="S15" s="1" t="s">
         <v>30</v>
       </c>
@@ -6776,9 +7568,9 @@
       <c r="D16" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="2">
         <v>8481692</v>
       </c>
@@ -6791,13 +7583,13 @@
       <c r="K16" s="2">
         <v>1</v>
       </c>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="12"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="2"/>
       <c r="S16" s="1" t="s">
         <v>30</v>
       </c>
@@ -6825,9 +7617,9 @@
       <c r="D17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
       <c r="H17" s="2">
         <v>8479973</v>
       </c>
@@ -6840,13 +7632,13 @@
       <c r="K17" s="2">
         <v>0</v>
       </c>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="12"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="2"/>
       <c r="S17" s="1" t="s">
         <v>30</v>
       </c>
@@ -6874,9 +7666,9 @@
       <c r="D18" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
       <c r="H18" s="2">
         <v>8480947</v>
       </c>
@@ -6889,13 +7681,13 @@
       <c r="K18" s="2">
         <v>1</v>
       </c>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="12"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="2"/>
       <c r="S18" s="1" t="s">
         <v>30</v>
       </c>
@@ -6923,9 +7715,9 @@
       <c r="D19" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
       <c r="H19" s="2">
         <v>8480313</v>
       </c>
@@ -6938,13 +7730,13 @@
       <c r="K19" s="2">
         <v>0</v>
       </c>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="12"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="2"/>
       <c r="S19" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
feat: fix and run
</commit_message>
<xml_diff>
--- a/betting_tracker.xlsx
+++ b/betting_tracker.xlsx
@@ -6144,152 +6144,126 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
-    <col width="10" customWidth="1" min="11" max="11"/>
-    <col width="15" customWidth="1" min="12" max="12"/>
-    <col width="12" customWidth="1" min="13" max="13"/>
-    <col width="14" customWidth="1" min="14" max="14"/>
-    <col width="16" customWidth="1" min="15" max="15"/>
-    <col width="15" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
-    <col width="12" customWidth="1" min="18" max="18"/>
-    <col width="14" customWidth="1" min="19" max="19"/>
-    <col width="13" customWidth="1" min="20" max="20"/>
-    <col width="10" customWidth="1" min="21" max="21"/>
-    <col width="12" customWidth="1" min="22" max="22"/>
-    <col width="30" customWidth="1" min="23" max="23"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="21" t="inlineStr">
+      <c r="A1" s="20" t="inlineStr">
         <is>
           <t>game_date</t>
         </is>
       </c>
-      <c r="B1" s="21" t="inlineStr">
+      <c r="B1" s="20" t="inlineStr">
         <is>
           <t>game_id</t>
         </is>
       </c>
-      <c r="C1" s="21" t="inlineStr">
+      <c r="C1" s="20" t="inlineStr">
         <is>
           <t>book</t>
         </is>
       </c>
-      <c r="D1" s="21" t="inlineStr">
+      <c r="D1" s="20" t="inlineStr">
         <is>
           <t>goalie_name</t>
         </is>
       </c>
-      <c r="E1" s="21" t="inlineStr">
+      <c r="E1" s="20" t="inlineStr">
         <is>
           <t>betting_line</t>
         </is>
       </c>
-      <c r="F1" s="21" t="inlineStr">
+      <c r="F1" s="20" t="inlineStr">
         <is>
           <t>line_over</t>
         </is>
       </c>
-      <c r="G1" s="21" t="inlineStr">
+      <c r="G1" s="20" t="inlineStr">
         <is>
           <t>line_under</t>
         </is>
       </c>
-      <c r="H1" s="21" t="inlineStr">
+      <c r="H1" s="20" t="inlineStr">
         <is>
           <t>goalie_id</t>
         </is>
       </c>
-      <c r="I1" s="21" t="inlineStr">
+      <c r="I1" s="20" t="inlineStr">
         <is>
           <t>team_abbrev</t>
         </is>
       </c>
-      <c r="J1" s="21" t="inlineStr">
+      <c r="J1" s="20" t="inlineStr">
         <is>
           <t>opponent_team</t>
         </is>
       </c>
-      <c r="K1" s="21" t="inlineStr">
+      <c r="K1" s="20" t="inlineStr">
         <is>
           <t>is_home</t>
         </is>
       </c>
-      <c r="L1" s="21" t="inlineStr">
+      <c r="L1" s="20" t="inlineStr">
         <is>
           <t>predicted_saves</t>
         </is>
       </c>
-      <c r="M1" s="21" t="inlineStr">
+      <c r="M1" s="20" t="inlineStr">
         <is>
           <t>prob_over</t>
         </is>
       </c>
-      <c r="N1" s="21" t="inlineStr">
+      <c r="N1" s="20" t="inlineStr">
         <is>
           <t>confidence_pct</t>
         </is>
       </c>
-      <c r="O1" s="21" t="inlineStr">
+      <c r="O1" s="20" t="inlineStr">
         <is>
           <t>confidence_bucket</t>
         </is>
       </c>
-      <c r="P1" s="21" t="inlineStr">
+      <c r="P1" s="20" t="inlineStr">
         <is>
           <t>recommendation</t>
         </is>
       </c>
-      <c r="Q1" s="21" t="inlineStr">
+      <c r="Q1" s="20" t="inlineStr">
         <is>
           <t>ev</t>
         </is>
       </c>
-      <c r="R1" s="21" t="inlineStr">
+      <c r="R1" s="20" t="inlineStr">
         <is>
           <t>bet_amount</t>
         </is>
       </c>
-      <c r="S1" s="21" t="inlineStr">
+      <c r="S1" s="20" t="inlineStr">
         <is>
           <t>bet_selection</t>
         </is>
       </c>
-      <c r="T1" s="21" t="inlineStr">
+      <c r="T1" s="20" t="inlineStr">
         <is>
           <t>actual_saves</t>
         </is>
       </c>
-      <c r="U1" s="21" t="inlineStr">
+      <c r="U1" s="20" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="V1" s="21" t="inlineStr">
+      <c r="V1" s="20" t="inlineStr">
         <is>
           <t>profit_loss</t>
         </is>
       </c>
-      <c r="W1" s="21" t="inlineStr">
+      <c r="W1" s="20" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
@@ -6309,6 +6283,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>TOR</t>
@@ -6353,6 +6328,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
           <t>VGK</t>
@@ -6397,6 +6373,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>CHI</t>
@@ -6441,6 +6418,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>TBL</t>
@@ -6485,6 +6463,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
           <t>DAL</t>
@@ -6529,6 +6508,7 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
           <t>STL</t>
@@ -6573,6 +6553,7 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
           <t>COL</t>
@@ -6617,6 +6598,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
           <t>PHI</t>
@@ -6661,6 +6643,7 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
           <t>CGY</t>
@@ -6705,6 +6688,7 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
           <t>WSH</t>
@@ -6749,6 +6733,7 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>VAN</t>
@@ -6793,6 +6778,7 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
           <t>NJD</t>
@@ -6837,6 +6823,7 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr">
         <is>
           <t>SJS</t>
@@ -6881,6 +6868,7 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
           <t>NYR</t>
@@ -6925,6 +6913,7 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
           <t>SEA</t>
@@ -6969,6 +6958,7 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
           <t>ANA</t>
@@ -6998,6 +6988,160 @@
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2025020802</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Underdog</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Stolarz</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-118</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-104</v>
+      </c>
+      <c r="H18" t="n">
+        <v>8476932</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>VGK</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>25.39999961853027</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.4886266887187958</v>
+      </c>
+      <c r="N18" t="n">
+        <v>2.274662256240845</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.00156933069229126</v>
+      </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2025020802</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>PrizePicks</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Stolarz</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-120</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-120</v>
+      </c>
+      <c r="H19" t="n">
+        <v>8476932</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>VGK</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" t="n">
+        <v>25.39999961853027</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.4886266887187958</v>
+      </c>
+      <c r="N19" t="n">
+        <v>2.274662256240845</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>50-55%</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>NO BET</t>
+        </is>
+      </c>
+      <c r="Q19" t="n">
+        <v>-0.03408128023147583</v>
+      </c>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: added model training guide
</commit_message>
<xml_diff>
--- a/betting_tracker.xlsx
+++ b/betting_tracker.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2470" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2494" uniqueCount="212">
   <si>
     <t>game_date</t>
   </si>
@@ -802,23 +802,23 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -7449,7 +7449,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -7472,7 +7472,7 @@
     <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -7481,73 +7481,73 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7555,7 +7555,7 @@
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="15">
         <v>2025020819</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -7564,16 +7564,16 @@
       <c r="D2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <v>28.5</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="15">
         <v>-125</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="15">
         <v>102</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="15">
         <v>8479361</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -7582,16 +7582,16 @@
       <c r="J2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="15">
         <v>1</v>
       </c>
-      <c r="L2" s="17">
+      <c r="L2" s="16">
         <v>28.39999961853027</v>
       </c>
-      <c r="M2" s="17">
+      <c r="M2" s="16">
         <v>0.4716980457305908</v>
       </c>
-      <c r="N2" s="17">
+      <c r="N2" s="16">
         <v>5.660390853881836</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -7600,10 +7600,10 @@
       <c r="P2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="Q2" s="16">
         <v>0.033252447843552</v>
       </c>
-      <c r="R2" s="12">
+      <c r="R2" s="15">
         <v>1</v>
       </c>
       <c r="S2" s="1" t="s">
@@ -7618,7 +7618,7 @@
       <c r="A3" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="15">
         <v>2025020820</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -7627,16 +7627,16 @@
       <c r="D3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>22.5</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="15">
         <v>-105</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="15">
         <v>-118</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="15">
         <v>8474593</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -7645,16 +7645,16 @@
       <c r="J3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="12">
-        <v>0</v>
-      </c>
-      <c r="L3" s="17">
+      <c r="K3" s="15">
+        <v>0</v>
+      </c>
+      <c r="L3" s="16">
         <v>22.70000076293945</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="16">
         <v>0.5359347462654114</v>
       </c>
-      <c r="N3" s="17">
+      <c r="N3" s="16">
         <v>7.186949253082275</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -7663,10 +7663,10 @@
       <c r="P3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="Q3" s="16">
         <v>0.02373963594436646</v>
       </c>
-      <c r="R3" s="12">
+      <c r="R3" s="15">
         <v>1</v>
       </c>
       <c r="S3" s="1" t="s">
@@ -7681,7 +7681,7 @@
       <c r="A4" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="15">
         <v>2025020823</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -7690,16 +7690,16 @@
       <c r="D4" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>21.5</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="15">
         <v>-103</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="15">
         <v>-121</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="15">
         <v>8480193</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -7708,16 +7708,16 @@
       <c r="J4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K4" s="12">
-        <v>0</v>
-      </c>
-      <c r="L4" s="17">
+      <c r="K4" s="15">
+        <v>0</v>
+      </c>
+      <c r="L4" s="16">
         <v>21.60000038146973</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="16">
         <v>0.5226746797561646</v>
       </c>
-      <c r="N4" s="17">
+      <c r="N4" s="16">
         <v>4.53493595123291</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -7726,10 +7726,10 @@
       <c r="P4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="17">
+      <c r="Q4" s="16">
         <v>0.015285491943359</v>
       </c>
-      <c r="R4" s="18"/>
+      <c r="R4" s="17"/>
       <c r="S4" s="1" t="s">
         <v>30</v>
       </c>
@@ -7742,7 +7742,7 @@
       <c r="A5" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="15">
         <v>2025020823</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -7751,16 +7751,16 @@
       <c r="D5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>25.5</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="15">
         <v>-120</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="15">
         <v>-104</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="15">
         <v>8481519</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -7769,16 +7769,16 @@
       <c r="J5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="15">
         <v>1</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="16">
         <v>25.39999961853027</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="16">
         <v>0.4776476323604584</v>
       </c>
-      <c r="N5" s="17">
+      <c r="N5" s="16">
         <v>4.470473289489746</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -7787,10 +7787,10 @@
       <c r="P5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="Q5" s="16">
         <v>0.012548387050629</v>
       </c>
-      <c r="R5" s="18"/>
+      <c r="R5" s="17"/>
       <c r="S5" s="1" t="s">
         <v>30</v>
       </c>
@@ -7803,7 +7803,7 @@
       <c r="A6" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="15">
         <v>2025020824</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -7812,16 +7812,16 @@
       <c r="D6" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>24.5</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="15">
         <v>-124</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="15">
         <v>101</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="15">
         <v>8481692</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -7830,16 +7830,16 @@
       <c r="J6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="15">
         <v>1</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="16">
         <v>24.5</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="16">
         <v>0.4943341314792633</v>
       </c>
-      <c r="N6" s="17">
+      <c r="N6" s="16">
         <v>1.133173704147339</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -7848,10 +7848,10 @@
       <c r="P6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="Q6" s="16">
         <v>0.008153468370438</v>
       </c>
-      <c r="R6" s="18"/>
+      <c r="R6" s="17"/>
       <c r="S6" s="1" t="s">
         <v>30</v>
       </c>
@@ -7864,7 +7864,7 @@
       <c r="A7" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="15">
         <v>2025020823</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -7873,16 +7873,16 @@
       <c r="D7" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>25.5</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="15">
         <v>-120</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="15">
         <v>-120</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="15">
         <v>8481519</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -7891,16 +7891,16 @@
       <c r="J7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="15">
         <v>1</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="16">
         <v>25.39999961853027</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="16">
         <v>0.4776476323604584</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="16">
         <v>4.470473289489746</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -7909,10 +7909,10 @@
       <c r="P7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="Q7" s="16">
         <v>-0.02310222387313843</v>
       </c>
-      <c r="R7" s="18"/>
+      <c r="R7" s="17"/>
       <c r="S7" s="1" t="s">
         <v>30</v>
       </c>
@@ -7925,7 +7925,7 @@
       <c r="A8" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="15">
         <v>2025020823</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -7934,16 +7934,16 @@
       <c r="D8" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>21.5</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="15">
         <v>-120</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="15">
         <v>-120</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="15">
         <v>8480193</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -7952,16 +7952,16 @@
       <c r="J8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="17">
+      <c r="K8" s="15">
+        <v>0</v>
+      </c>
+      <c r="L8" s="16">
         <v>21.60000038146973</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="16">
         <v>0.5226746797561646</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="16">
         <v>4.53493595123291</v>
       </c>
       <c r="O8" s="1" t="s">
@@ -7970,10 +7970,10 @@
       <c r="P8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="16">
         <v>-0.02277988195419312</v>
       </c>
-      <c r="R8" s="18"/>
+      <c r="R8" s="17"/>
       <c r="S8" s="1" t="s">
         <v>30</v>
       </c>
@@ -7986,7 +7986,7 @@
       <c r="A9" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="15">
         <v>2025020824</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -7995,16 +7995,16 @@
       <c r="D9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>24.5</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="15">
         <v>-120</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="15">
         <v>-120</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="15">
         <v>8481692</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -8013,16 +8013,16 @@
       <c r="J9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="15">
         <v>1</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="16">
         <v>24.5</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="16">
         <v>0.4943341314792633</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N9" s="16">
         <v>1.133173704147339</v>
       </c>
       <c r="O9" s="1" t="s">
@@ -8031,10 +8031,10 @@
       <c r="P9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="17">
+      <c r="Q9" s="16">
         <v>-0.03978866338729858</v>
       </c>
-      <c r="R9" s="18"/>
+      <c r="R9" s="17"/>
       <c r="S9" s="1" t="s">
         <v>30</v>
       </c>
@@ -8047,7 +8047,7 @@
       <c r="A10" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="15">
         <v>2025020819</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -8056,16 +8056,16 @@
       <c r="D10" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>28.5</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="15">
         <v>-145</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="15">
         <v>112</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="15">
         <v>8479361</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -8074,16 +8074,16 @@
       <c r="J10" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="15">
         <v>1</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="16">
         <v>28.39999961853027</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="16">
         <v>0.4716980457305908</v>
       </c>
-      <c r="N10" s="17">
+      <c r="N10" s="16">
         <v>5.660390853881836</v>
       </c>
       <c r="O10" s="1" t="s">
@@ -8092,10 +8092,10 @@
       <c r="P10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Q10" s="17">
+      <c r="Q10" s="16">
         <v>0.05660384893417358</v>
       </c>
-      <c r="R10" s="12">
+      <c r="R10" s="15">
         <v>2</v>
       </c>
       <c r="S10" s="1" t="s">
@@ -8110,7 +8110,7 @@
       <c r="A11" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="15">
         <v>2025020819</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -8119,16 +8119,16 @@
       <c r="D11" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <v>22.5</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="15">
         <v>-106</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="15">
         <v>-117</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="15">
         <v>8478406</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -8137,16 +8137,16 @@
       <c r="J11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="12">
-        <v>0</v>
-      </c>
-      <c r="L11" s="17">
+      <c r="K11" s="15">
+        <v>0</v>
+      </c>
+      <c r="L11" s="16">
         <v>22.70000076293945</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="16">
         <v>0.5326666235923767</v>
       </c>
-      <c r="N11" s="17">
+      <c r="N11" s="16">
         <v>6.533324718475342</v>
       </c>
       <c r="O11" s="1" t="s">
@@ -8155,10 +8155,10 @@
       <c r="P11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q11" s="17">
+      <c r="Q11" s="16">
         <v>0.018103539943695</v>
       </c>
-      <c r="R11" s="18"/>
+      <c r="R11" s="17"/>
       <c r="S11" s="1" t="s">
         <v>30</v>
       </c>
@@ -8171,7 +8171,7 @@
       <c r="A12" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="15">
         <v>2025020820</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -8180,16 +8180,16 @@
       <c r="D12" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>22.5</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="15">
         <v>-120</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="15">
         <v>-120</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="15">
         <v>8474593</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -8198,16 +8198,16 @@
       <c r="J12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="12">
-        <v>0</v>
-      </c>
-      <c r="L12" s="17">
+      <c r="K12" s="15">
+        <v>0</v>
+      </c>
+      <c r="L12" s="16">
         <v>22.70000076293945</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="16">
         <v>0.5359347462654114</v>
       </c>
-      <c r="N12" s="17">
+      <c r="N12" s="16">
         <v>7.186949253082275</v>
       </c>
       <c r="O12" s="1" t="s">
@@ -8216,10 +8216,10 @@
       <c r="P12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q12" s="17">
-        <v>-0.009519815444946289</v>
-      </c>
-      <c r="R12" s="18"/>
+      <c r="Q12" s="16">
+        <v>-0.009519815444946</v>
+      </c>
+      <c r="R12" s="17"/>
       <c r="S12" s="1" t="s">
         <v>30</v>
       </c>
@@ -8227,6 +8227,191 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="15">
+        <v>2025020819</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="16">
+        <v>22.5</v>
+      </c>
+      <c r="F13" s="15">
+        <v>-120</v>
+      </c>
+      <c r="G13" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H13" s="15">
+        <v>8478406</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="15">
+        <v>0</v>
+      </c>
+      <c r="L13" s="16">
+        <v>22.70000076293945</v>
+      </c>
+      <c r="M13" s="16">
+        <v>0.5326666235923767</v>
+      </c>
+      <c r="N13" s="16">
+        <v>6.533324718475342</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>-0.012787938117981</v>
+      </c>
+      <c r="R13" s="17"/>
+      <c r="S13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="15">
+        <v>2025020819</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="16">
+        <v>22.5</v>
+      </c>
+      <c r="F14" s="15">
+        <v>-109</v>
+      </c>
+      <c r="G14" s="15">
+        <v>-119</v>
+      </c>
+      <c r="H14" s="15">
+        <v>8478406</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="15">
+        <v>0</v>
+      </c>
+      <c r="L14" s="16">
+        <v>22.70000076293945</v>
+      </c>
+      <c r="M14" s="16">
+        <v>0.5326666235923767</v>
+      </c>
+      <c r="N14" s="16">
+        <v>6.533324718475342</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>0.0111355185508728</v>
+      </c>
+      <c r="R14" s="17"/>
+      <c r="S14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="15">
+        <v>2025020820</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="16">
+        <v>22.5</v>
+      </c>
+      <c r="F15" s="15">
+        <v>-108</v>
+      </c>
+      <c r="G15" s="15">
+        <v>-120</v>
+      </c>
+      <c r="H15" s="15">
+        <v>8474593</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="16">
+        <v>22.70000076293945</v>
+      </c>
+      <c r="M15" s="16">
+        <v>0.5359347462654114</v>
+      </c>
+      <c r="N15" s="16">
+        <v>7.186949253082275</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>0.016703963279724</v>
+      </c>
+      <c r="R15" s="17">
+        <v>1</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8261,7 +8446,7 @@
     <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -8461,7 +8646,7 @@
       <c r="Q3" s="3">
         <v>-0.01456844806671143</v>
       </c>
-      <c r="R3" s="12"/>
+      <c r="R3" s="2"/>
       <c r="S3" s="1" t="s">
         <v>30</v>
       </c>
@@ -8528,7 +8713,7 @@
       <c r="Q4" s="3">
         <v>-0.01076918840408325</v>
       </c>
-      <c r="R4" s="12"/>
+      <c r="R4" s="2"/>
       <c r="S4" s="1" t="s">
         <v>30</v>
       </c>
@@ -8595,7 +8780,7 @@
       <c r="Q5" s="3">
         <v>-0.01323801279067993</v>
       </c>
-      <c r="R5" s="12"/>
+      <c r="R5" s="2"/>
       <c r="S5" s="1" t="s">
         <v>30</v>
       </c>
@@ -8731,7 +8916,7 @@
       <c r="Q7" s="3">
         <v>0.003418862819671631</v>
       </c>
-      <c r="R7" s="12"/>
+      <c r="R7" s="2"/>
       <c r="S7" s="1" t="s">
         <v>30</v>
       </c>
@@ -8798,7 +8983,7 @@
       <c r="Q8" s="3">
         <v>0.01165533065795898</v>
       </c>
-      <c r="R8" s="12"/>
+      <c r="R8" s="2"/>
       <c r="S8" s="1" t="s">
         <v>30</v>
       </c>
@@ -9003,7 +9188,7 @@
       <c r="Q11" s="3">
         <v>-0.01742786169052124</v>
       </c>
-      <c r="R11" s="12"/>
+      <c r="R11" s="2"/>
       <c r="S11" s="1" t="s">
         <v>30</v>
       </c>
@@ -9070,7 +9255,7 @@
       <c r="Q12" s="3">
         <v>-0.02628129720687866</v>
       </c>
-      <c r="R12" s="12"/>
+      <c r="R12" s="2"/>
       <c r="S12" s="1" t="s">
         <v>30</v>
       </c>
@@ -9137,7 +9322,7 @@
       <c r="Q13" s="3">
         <v>0.003040581941604614</v>
       </c>
-      <c r="R13" s="12"/>
+      <c r="R13" s="2"/>
       <c r="S13" s="1" t="s">
         <v>30</v>
       </c>
@@ -9204,7 +9389,7 @@
       <c r="Q14" s="3">
         <v>0.005803912878036499</v>
       </c>
-      <c r="R14" s="12"/>
+      <c r="R14" s="2"/>
       <c r="S14" s="1" t="s">
         <v>30</v>
       </c>
@@ -9271,7 +9456,7 @@
       <c r="Q15" s="3">
         <v>-0.02239546179771423</v>
       </c>
-      <c r="R15" s="12"/>
+      <c r="R15" s="2"/>
       <c r="S15" s="1" t="s">
         <v>30</v>
       </c>
@@ -9338,7 +9523,7 @@
       <c r="Q16" s="3">
         <v>-0.01233145594596863</v>
       </c>
-      <c r="R16" s="12"/>
+      <c r="R16" s="2"/>
       <c r="S16" s="1" t="s">
         <v>30</v>
       </c>
@@ -9405,7 +9590,7 @@
       <c r="Q17" s="3">
         <v>-0.03937101364135742</v>
       </c>
-      <c r="R17" s="12"/>
+      <c r="R17" s="2"/>
       <c r="S17" s="1" t="s">
         <v>30</v>
       </c>
@@ -9472,7 +9657,7 @@
       <c r="Q18" s="3">
         <v>-0.02799868583679199</v>
       </c>
-      <c r="R18" s="12"/>
+      <c r="R18" s="2"/>
       <c r="S18" s="1" t="s">
         <v>30</v>
       </c>
@@ -9539,7 +9724,7 @@
       <c r="Q19" s="3">
         <v>-0.01643240451812744</v>
       </c>
-      <c r="R19" s="12"/>
+      <c r="R19" s="2"/>
       <c r="S19" s="1" t="s">
         <v>30</v>
       </c>
@@ -9606,7 +9791,7 @@
       <c r="Q20" s="3">
         <v>-0.02183997631072998</v>
       </c>
-      <c r="R20" s="12"/>
+      <c r="R20" s="2"/>
       <c r="S20" s="1" t="s">
         <v>30</v>
       </c>
@@ -9673,7 +9858,7 @@
       <c r="Q21" s="3">
         <v>-0.03045147657394409</v>
       </c>
-      <c r="R21" s="12"/>
+      <c r="R21" s="2"/>
       <c r="S21" s="1" t="s">
         <v>30</v>
       </c>
@@ -9740,7 +9925,7 @@
       <c r="Q22" s="3">
         <v>-0.0446588397026062</v>
       </c>
-      <c r="R22" s="12"/>
+      <c r="R22" s="2"/>
       <c r="S22" s="1" t="s">
         <v>30</v>
       </c>
@@ -9807,7 +9992,7 @@
       <c r="Q23" s="3">
         <v>-0.04354465007781982</v>
       </c>
-      <c r="R23" s="12"/>
+      <c r="R23" s="2"/>
       <c r="S23" s="1" t="s">
         <v>30</v>
       </c>
@@ -9874,7 +10059,7 @@
       <c r="Q24" s="3">
         <v>-0.02057152986526489</v>
       </c>
-      <c r="R24" s="12"/>
+      <c r="R24" s="2"/>
       <c r="S24" s="1" t="s">
         <v>30</v>
       </c>
@@ -9941,7 +10126,7 @@
       <c r="Q25" s="3">
         <v>-0.04531818628311157</v>
       </c>
-      <c r="R25" s="12"/>
+      <c r="R25" s="2"/>
       <c r="S25" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>